<commit_message>
readtablesfromexcel now has filename as argument.
</commit_message>
<xml_diff>
--- a/DCC-Table_example3.xlsx
+++ b/DCC-Table_example3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\1901 NY-INFRA-FOT\DCC\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D2A2AA-FFAF-40D8-B0DD-2F4FFF3D6CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13E4CA0-302E-40E8-AC96-B5399B5CA157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="37220" windowHeight="21820" activeTab="2" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="21220" windowHeight="14770" activeTab="2" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="83">
   <si>
     <t>customerTag</t>
   </si>
@@ -277,6 +277,21 @@
   </si>
   <si>
     <t>UncertaintyCoverageProbability</t>
+  </si>
+  <si>
+    <t>scope</t>
+  </si>
+  <si>
+    <t>measurand</t>
+  </si>
+  <si>
+    <t>dataCategory</t>
+  </si>
+  <si>
+    <t>Indicated resistance of the calibration item</t>
+  </si>
+  <si>
+    <t>Accreditation applies</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5683CA04-207D-4144-92F8-9A8A86CEED7F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
@@ -1093,19 +1108,19 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
     <col min="2" max="2" width="12.26953125" customWidth="1"/>
     <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.54296875" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" customWidth="1"/>
-    <col min="8" max="8" width="13.90625" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="14.54296875" customWidth="1"/>
     <col min="11" max="11" width="13.7265625" customWidth="1"/>
@@ -1154,7 +1169,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>34</v>
@@ -1187,7 +1202,7 @@
         <v>35</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="M6" s="12" t="s">
         <v>34</v>
@@ -1195,7 +1210,7 @@
     </row>
     <row r="7" spans="1:13" ht="22">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>0</v>
@@ -1236,7 +1251,7 @@
     </row>
     <row r="8" spans="1:13" ht="22">
       <c r="A8" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>37</v>
@@ -1312,7 +1327,7 @@
       </c>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" ht="22">
+    <row r="10" spans="1:13" ht="32.5">
       <c r="A10" s="11" t="s">
         <v>61</v>
       </c>
@@ -1345,10 +1360,10 @@
         <v>51</v>
       </c>
       <c r="L10" s="24" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="M10" s="23" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1362,8 +1377,8 @@
         <v>0</v>
       </c>
       <c r="D11" s="19">
-        <f>E11+273.15</f>
-        <v>273.15999999999997</v>
+        <f>ROUND(E11+273.15,2)</f>
+        <v>273.16000000000003</v>
       </c>
       <c r="E11" s="19">
         <v>0.01</v>
@@ -1372,8 +1387,8 @@
         <v>-0.1</v>
       </c>
       <c r="G11" s="9">
-        <f>F11-E11</f>
-        <v>-0.11</v>
+        <f>ROUND(F11-E11,1)</f>
+        <v>-0.1</v>
       </c>
       <c r="H11" s="25">
         <v>0.05</v>
@@ -1405,8 +1420,8 @@
         <v>15</v>
       </c>
       <c r="D12" s="19">
-        <f>E12+273.15</f>
-        <v>288.15999999999997</v>
+        <f t="shared" ref="D12:D15" si="0">ROUND(E12+273.15,2)</f>
+        <v>288.16000000000003</v>
       </c>
       <c r="E12" s="19">
         <v>15.01</v>
@@ -1415,8 +1430,8 @@
         <v>15.1</v>
       </c>
       <c r="G12" s="9">
-        <f t="shared" ref="G12:G15" si="0">F12-E12</f>
-        <v>8.9999999999999858E-2</v>
+        <f t="shared" ref="G12:G15" si="1">ROUND(F12-E12,1)</f>
+        <v>0.1</v>
       </c>
       <c r="H12" s="25">
         <v>0.05</v>
@@ -1448,8 +1463,8 @@
         <v>25</v>
       </c>
       <c r="D13" s="19">
-        <f>E13+273.15</f>
-        <v>298.16999999999996</v>
+        <f t="shared" si="0"/>
+        <v>298.17</v>
       </c>
       <c r="E13" s="19">
         <v>25.02</v>
@@ -1458,8 +1473,8 @@
         <v>25.2</v>
       </c>
       <c r="G13" s="9">
-        <f t="shared" si="0"/>
-        <v>0.17999999999999972</v>
+        <f t="shared" si="1"/>
+        <v>0.2</v>
       </c>
       <c r="H13" s="25">
         <v>0.05</v>
@@ -1491,8 +1506,8 @@
         <v>15</v>
       </c>
       <c r="D14" s="19">
-        <f>E14+273.15</f>
-        <v>288.15999999999997</v>
+        <f t="shared" si="0"/>
+        <v>288.16000000000003</v>
       </c>
       <c r="E14" s="19">
         <v>15.01</v>
@@ -1501,8 +1516,8 @@
         <v>15.3</v>
       </c>
       <c r="G14" s="9">
-        <f t="shared" si="0"/>
-        <v>0.29000000000000092</v>
+        <f t="shared" si="1"/>
+        <v>0.3</v>
       </c>
       <c r="H14" s="25">
         <v>0.05</v>
@@ -1533,9 +1548,9 @@
       <c r="C15" s="21">
         <v>0</v>
       </c>
-      <c r="D15" s="22">
-        <f>E15+273.15</f>
-        <v>273.15999999999997</v>
+      <c r="D15" s="19">
+        <f t="shared" si="0"/>
+        <v>273.16000000000003</v>
       </c>
       <c r="E15" s="22">
         <v>0.01</v>
@@ -1543,9 +1558,9 @@
       <c r="F15" s="7">
         <v>0</v>
       </c>
-      <c r="G15" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.01</v>
+      <c r="G15" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="H15" s="25">
         <v>0.05</v>
@@ -1569,7 +1584,7 @@
   </sheetData>
   <dataConsolidate/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:M8" xr:uid="{01692EB9-2CFF-4754-B166-4E8AFE51A7B5}">
       <formula1>MeasurandType</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Excel Example 3 er opdateret
</commit_message>
<xml_diff>
--- a/DCC-Table_example3.xlsx
+++ b/DCC-Table_example3.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\1901 NY-INFRA-FOT\DCC\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13E4CA0-302E-40E8-AC96-B5399B5CA157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF116E4-78D6-40FD-8DA5-6CE0C9E04024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="21220" windowHeight="14770" activeTab="2" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
+    <workbookView xWindow="2670" yWindow="2540" windowWidth="25560" windowHeight="14770" activeTab="2" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
     <sheet name="AdministrativeData" sheetId="4" r:id="rId2"/>
-    <sheet name="Table2" sheetId="5" r:id="rId3"/>
+    <sheet name="Statements" sheetId="6" r:id="rId3"/>
+    <sheet name="Items" sheetId="7" r:id="rId4"/>
+    <sheet name="Table2" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="ColType">Definitions!$H$3:$H$7</definedName>
-    <definedName name="MeasurandType">Definitions!$K$3:$K$46</definedName>
-    <definedName name="MetaType">Definitions!$D$3:$D$22</definedName>
+    <definedName name="ColType">Definitions!$A$3:$A$7</definedName>
+    <definedName name="MeasurandType">Definitions!$C$3:$C$46</definedName>
+    <definedName name="MetaType">Definitions!$B$3:$B$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="190">
   <si>
     <t>customerTag</t>
   </si>
@@ -183,9 +185,6 @@
     <t>UsedEquipment</t>
   </si>
   <si>
-    <t>ColumnType</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -255,9 +254,6 @@
     <t>data_row5</t>
   </si>
   <si>
-    <t>scopeType</t>
-  </si>
-  <si>
     <t>numRows</t>
   </si>
   <si>
@@ -292,6 +288,333 @@
   </si>
   <si>
     <t>Accreditation applies</t>
+  </si>
+  <si>
+    <t>scopeTypes</t>
+  </si>
+  <si>
+    <t>dataCategoryType</t>
+  </si>
+  <si>
+    <t>UserLabel</t>
+  </si>
+  <si>
+    <t>DFM_Software_Name</t>
+  </si>
+  <si>
+    <t>DFM substituter</t>
+  </si>
+  <si>
+    <t>DFM_Software_Version</t>
+  </si>
+  <si>
+    <t>v0.0.1</t>
+  </si>
+  <si>
+    <t>DFM_Unique_ID</t>
+  </si>
+  <si>
+    <t>DFM-T220000</t>
+  </si>
+  <si>
+    <t>Certificate_no</t>
+  </si>
+  <si>
+    <t>DFM_CertificateNo</t>
+  </si>
+  <si>
+    <t>DFM_OrderNo</t>
+  </si>
+  <si>
+    <t>8000650430</t>
+  </si>
+  <si>
+    <t>DFM_ArrivalDate</t>
+  </si>
+  <si>
+    <t>2022-02-18</t>
+  </si>
+  <si>
+    <t>DFM_StartDate</t>
+  </si>
+  <si>
+    <t>2022-02-21</t>
+  </si>
+  <si>
+    <t>Calibr_date</t>
+  </si>
+  <si>
+    <t>DFM_EndDate</t>
+  </si>
+  <si>
+    <t>2022-02-22</t>
+  </si>
+  <si>
+    <t>DFM_Item1_Description</t>
+  </si>
+  <si>
+    <t>Digitaltermometer</t>
+  </si>
+  <si>
+    <t>DFM_Item1_Name</t>
+  </si>
+  <si>
+    <t>Fluke</t>
+  </si>
+  <si>
+    <t>DFM_Item1_Maufacturer</t>
+  </si>
+  <si>
+    <t>Temperature sensor</t>
+  </si>
+  <si>
+    <t>DFM_Item1_Model</t>
+  </si>
+  <si>
+    <t>1523</t>
+  </si>
+  <si>
+    <t>DFM_Item1_SerialNo</t>
+  </si>
+  <si>
+    <t>8864333</t>
+  </si>
+  <si>
+    <t>Id_no</t>
+  </si>
+  <si>
+    <t>DFM_Item1_ID</t>
+  </si>
+  <si>
+    <t>DMC-2769</t>
+  </si>
+  <si>
+    <t>Supplier_Name</t>
+  </si>
+  <si>
+    <t>DFM_CalLab_CompanyName</t>
+  </si>
+  <si>
+    <t>DFM A/S</t>
+  </si>
+  <si>
+    <t>DFM_CalLab_Email</t>
+  </si>
+  <si>
+    <t>Administration@dfm.dk</t>
+  </si>
+  <si>
+    <t>DFM_CalLab_Phone</t>
+  </si>
+  <si>
+    <t>+45 7730 5800</t>
+  </si>
+  <si>
+    <t>DFM_CalLab_City</t>
+  </si>
+  <si>
+    <t>Hørsholm</t>
+  </si>
+  <si>
+    <t>DFM_CalLab_Country</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>DFM_CalLab_PostalCode</t>
+  </si>
+  <si>
+    <t>2970</t>
+  </si>
+  <si>
+    <t>DFM_CalLab_Street1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kogle Alle </t>
+  </si>
+  <si>
+    <t>DFM_CalLab_Street_No</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>DFM_CalLab_Webpage</t>
+  </si>
+  <si>
+    <t>www.dfm.dk</t>
+  </si>
+  <si>
+    <t>DFM_SignedBy</t>
+  </si>
+  <si>
+    <t>J. S. Nielsen</t>
+  </si>
+  <si>
+    <t>DFM_Customer_CompanyName</t>
+  </si>
+  <si>
+    <t>Danish Measurement Company Ltd.</t>
+  </si>
+  <si>
+    <t>DFM_Customer_Email</t>
+  </si>
+  <si>
+    <t>mm@dmc.dk</t>
+  </si>
+  <si>
+    <t>DFM_Customer_City</t>
+  </si>
+  <si>
+    <t>Måløv</t>
+  </si>
+  <si>
+    <t>DFM_Customer_Country</t>
+  </si>
+  <si>
+    <t>DFM_Customer_PostalCode</t>
+  </si>
+  <si>
+    <t>9899</t>
+  </si>
+  <si>
+    <t>DFM_Customer_CompanyStreet1</t>
+  </si>
+  <si>
+    <t>Målervej</t>
+  </si>
+  <si>
+    <t>DFM_Customer_CompanyStreet_No</t>
+  </si>
+  <si>
+    <t>16, 1. sal</t>
+  </si>
+  <si>
+    <t>DFM_Customer_Att</t>
+  </si>
+  <si>
+    <t>Mads Målermand</t>
+  </si>
+  <si>
+    <t>DFM_Accreditation_CALRegNo</t>
+  </si>
+  <si>
+    <t>DK-255</t>
+  </si>
+  <si>
+    <t>DFM_Accreditation_traceable</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>DFM_Accreditation_valid</t>
+  </si>
+  <si>
+    <t>DFM_Accreditation_Statement</t>
+  </si>
+  <si>
+    <t>The calibration is performed under DANAK accreditation no. 255.\nDANAK is one of the signatories ot the EA Multilateral Agreement and the ILAC multilateral agreement for the mutual recognition of calibration certificates.</t>
+  </si>
+  <si>
+    <t>DFM_Accreditation_Body</t>
+  </si>
+  <si>
+    <t>DANAK</t>
+  </si>
+  <si>
+    <t>DFM_TermsOfUse_Statement</t>
+  </si>
+  <si>
+    <t>This certificate may not be reproduced except in full without the written approval of the laboratory.</t>
+  </si>
+  <si>
+    <t>DFM_Item1_Result1_Name_en</t>
+  </si>
+  <si>
+    <t>Temperatures accordign to ITS-90</t>
+  </si>
+  <si>
+    <t>DFM_Item1_Result1_Name_da</t>
+  </si>
+  <si>
+    <t>Temperaturer i henhold til ITS-90</t>
+  </si>
+  <si>
+    <t>DFM_Procedure</t>
+  </si>
+  <si>
+    <t>DFM proceedure Q2KAL251</t>
+  </si>
+  <si>
+    <t>DFM_Reference1_name</t>
+  </si>
+  <si>
+    <t>Standard Platinum Resistance Thermometer</t>
+  </si>
+  <si>
+    <t>DFM_Reference1_manufacturer</t>
+  </si>
+  <si>
+    <t>Rosemount</t>
+  </si>
+  <si>
+    <t>DFM_Reference1_model</t>
+  </si>
+  <si>
+    <t>162CE</t>
+  </si>
+  <si>
+    <t>DFM_Reference1_serial</t>
+  </si>
+  <si>
+    <t>5091</t>
+  </si>
+  <si>
+    <t>DFM_Reference1_ID</t>
+  </si>
+  <si>
+    <t>DFM-1546</t>
+  </si>
+  <si>
+    <t>DFM_Reference_Statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature is measured via DFM resistancethermometer Rosemount CE162/5091, with DFM calibration certificate number TIR2015. The calibration is executed in situ. </t>
+  </si>
+  <si>
+    <t>DFM_LabTemperature_Description</t>
+  </si>
+  <si>
+    <t>The calibrations are made at constant temperatures by comparison wiht laboratory standards traceable to SI.</t>
+  </si>
+  <si>
+    <t>DFM_LabTemperature_Value</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>DFM_LabTemperature_Unit</t>
+  </si>
+  <si>
+    <t>\degreeCelcius</t>
+  </si>
+  <si>
+    <t>DFM_LabTemperature_U</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>DFM_Item1_Norm</t>
+  </si>
+  <si>
+    <t>DKD-R 5-1:2018</t>
+  </si>
+  <si>
+    <t>Template Label</t>
   </si>
 </sst>
 </file>
@@ -301,7 +624,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,6 +674,14 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -490,12 +821,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -574,10 +906,14 @@
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
     <cellStyle name="40% - Accent6" xfId="1" builtinId="51"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -890,199 +1226,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F9C957-7C4E-4161-9FBF-0EC69D9D67E3}">
-  <dimension ref="D2:L21"/>
+  <dimension ref="A2:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="4:12">
-      <c r="D2" s="3" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="4:12">
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="4:12">
-      <c r="D4" t="s">
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
         <v>42</v>
       </c>
-      <c r="H4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="4:12">
-      <c r="D5" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="H5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="4:12">
-      <c r="D6" t="s">
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="H6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="4:12">
-      <c r="D7" t="s">
+    <row r="7" spans="1:12">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="K7" t="s">
+      <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="4:12">
-      <c r="D8" t="s">
+    <row r="8" spans="1:12">
+      <c r="A8" s="2"/>
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="K8" t="s">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="4:12">
-      <c r="D9" t="s">
+    <row r="9" spans="1:12">
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="K9" t="s">
+      <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="4:12">
-      <c r="D10" t="s">
+    <row r="10" spans="1:12">
+      <c r="B10" t="s">
         <v>43</v>
       </c>
-      <c r="K10" t="s">
+      <c r="C10" t="s">
         <v>16</v>
       </c>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="4:12">
-      <c r="D11" t="s">
+    <row r="11" spans="1:12">
+      <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="K11" t="s">
+      <c r="C11" t="s">
         <v>17</v>
       </c>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="4:12">
-      <c r="D12" t="s">
+    <row r="12" spans="1:12">
+      <c r="B12" t="s">
         <v>45</v>
       </c>
-      <c r="K12" t="s">
+      <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="4:12">
-      <c r="D13" t="s">
+    <row r="13" spans="1:12">
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="K13" t="s">
+      <c r="C13" t="s">
         <v>19</v>
       </c>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="4:12">
-      <c r="D14" t="s">
+    <row r="14" spans="1:12">
+      <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="K14" t="s">
+      <c r="C14" t="s">
         <v>20</v>
       </c>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="4:12">
-      <c r="D15" t="s">
+    <row r="15" spans="1:12">
+      <c r="B15" t="s">
         <v>0</v>
       </c>
-      <c r="K15" t="s">
+      <c r="C15" t="s">
         <v>21</v>
       </c>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="4:12">
-      <c r="D16" t="s">
+    <row r="16" spans="1:12">
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="K16" t="s">
+      <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="4:12">
-      <c r="D17" t="s">
+    <row r="17" spans="2:12">
+      <c r="B17" t="s">
         <v>41</v>
       </c>
-      <c r="K17" t="s">
+      <c r="C17" t="s">
         <v>3</v>
       </c>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="4:12">
-      <c r="D18" t="s">
-        <v>73</v>
-      </c>
-      <c r="K18" t="s">
+    <row r="18" spans="2:12">
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="4:12">
-      <c r="D19" t="s">
-        <v>74</v>
-      </c>
-      <c r="K19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="4:12">
-      <c r="D20" t="s">
-        <v>77</v>
-      </c>
-      <c r="K20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="4:12">
-      <c r="K21" t="s">
+    <row r="19" spans="2:12">
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="C21" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1093,9 +1434,474 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5683CA04-207D-4144-92F8-9A8A86CEED7F}">
+  <dimension ref="A1:C53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" t="s">
+        <v>152</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" t="s">
+        <v>154</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" t="s">
+        <v>161</v>
+      </c>
+      <c r="C40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" t="s">
+        <v>163</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" t="s">
+        <v>165</v>
+      </c>
+      <c r="C42" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" t="s">
+        <v>169</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="B46" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" t="s">
+        <v>177</v>
+      </c>
+      <c r="C48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" t="s">
+        <v>179</v>
+      </c>
+      <c r="C49" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" t="s">
+        <v>181</v>
+      </c>
+      <c r="C50" s="28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" t="s">
+        <v>183</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" t="s">
+        <v>185</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" t="s">
+        <v>187</v>
+      </c>
+      <c r="C53" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C23" r:id="rId1" display="www.dfm.dk" xr:uid="{E465C636-D594-413A-8B1A-468AA9848358}"/>
+    <hyperlink ref="C17" r:id="rId2" xr:uid="{924EC528-40C3-4804-BF99-CB9DC88AD4BA}"/>
+    <hyperlink ref="C24" r:id="rId3" xr:uid="{A9AAC80D-9488-47F1-80E3-8644FDD89076}"/>
+    <hyperlink ref="C27" r:id="rId4" xr:uid="{AC76966B-0028-4873-8565-AED87429289E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C531791-9242-4867-B027-97236DF4A138}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
@@ -1103,11 +1909,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181308C0-D531-4746-B510-8FF554CEB31C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C24526-8286-4257-8B46-E195D4F721E3}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -1130,28 +1948,28 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17.25" customHeight="1">
       <c r="A2" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="27">
         <f>COUNTA(A11:A1048576)</f>
@@ -1160,7 +1978,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" s="27">
         <f>COUNTA(B6:XFD6)</f>
@@ -1169,7 +1987,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>34</v>
@@ -1210,7 +2028,7 @@
     </row>
     <row r="7" spans="1:13" ht="22">
       <c r="A7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>0</v>
@@ -1219,22 +2037,22 @@
         <v>42</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>5</v>
@@ -1243,7 +2061,7 @@
         <v>6</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M7" s="12" t="s">
         <v>41</v>
@@ -1251,7 +2069,7 @@
     </row>
     <row r="8" spans="1:13" ht="22">
       <c r="A8" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>37</v>
@@ -1284,7 +2102,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M8" s="12" t="s">
         <v>37</v>
@@ -1292,7 +2110,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="15" t="s">
@@ -1320,16 +2138,16 @@
         <v>22</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:13" ht="32.5">
       <c r="A10" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="23" t="s">
@@ -1348,27 +2166,27 @@
         <v>32</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K10" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L10" s="24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M10" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>27</v>
@@ -1400,18 +2218,18 @@
         <v>0.2</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L11" s="8">
         <v>1</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>28</v>
@@ -1443,18 +2261,18 @@
         <v>0.2</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L12" s="8">
         <v>2</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>29</v>
@@ -1486,18 +2304,18 @@
         <v>0.2</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L13" s="8">
         <v>3</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>30</v>
@@ -1529,18 +2347,18 @@
         <v>0.2</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L14" s="8">
         <v>4</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>31</v>
@@ -1572,13 +2390,13 @@
         <v>0.2</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L15" s="4">
         <v>5</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Administrative data har nu XPATHs
</commit_message>
<xml_diff>
--- a/DCC-Table_example3.xlsx
+++ b/DCC-Table_example3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\1901 NY-INFRA-FOT\DCC\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF116E4-78D6-40FD-8DA5-6CE0C9E04024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2E124D-864F-42E9-8DC5-D621D4FE4E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="2540" windowWidth="25560" windowHeight="14770" activeTab="2" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
+    <workbookView xWindow="2960" yWindow="2960" windowWidth="25560" windowHeight="14770" activeTab="1" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="272">
   <si>
     <t>customerTag</t>
   </si>
@@ -615,6 +615,252 @@
   </si>
   <si>
     <t>Template Label</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>equipmentClass</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>swRef</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Customer ID</t>
+  </si>
+  <si>
+    <t>Product number</t>
+  </si>
+  <si>
+    <t>Serial number</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>countryCodeISO3166_1</t>
+  </si>
+  <si>
+    <t>convention</t>
+  </si>
+  <si>
+    <t>traceable</t>
+  </si>
+  <si>
+    <t>norm</t>
+  </si>
+  <si>
+    <t>declaration</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>preiod</t>
+  </si>
+  <si>
+    <t>respAuthority</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>nonSIDefinition</t>
+  </si>
+  <si>
+    <t>nonSIUnits</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>XPATH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:dccSoftware/dcc:software/dcc:name/dcc:content</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:dccSoftware/dcc:software/dcc:release</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:uniqueIdentifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:identifications/dcc:identification[1]/dcc:value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:identifications/dcc:identification[2]/dcc:value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:receiptDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:beginPerformanceDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:endPerformanceDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:items/dcc:name/dcc:content[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:items/dcc:item/dcc:name/dcc:content[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:items/dcc:item/dcc:manufacturer/dcc:name/dcc:content</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:items/dcc:item/dcc:model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:items/dcc:item/dcc:identifications/dcc:identification[1]/dcc:value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:items/dcc:item/dcc:identifications/dcc:identification[2]/dcc:value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:calibrationLaboratory/dcc:contact/dcc:name/dcc:content</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:calibrationLaboratory/dcc:contact/dcc:eMail</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:calibrationLaboratory/dcc:contact/dcc:phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:calibrationLaboratory/dcc:contact/dcc:location/dcc:city</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:calibrationLaboratory/dcc:contact/dcc:location/dcc:countryCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:calibrationLaboratory/dcc:contact/dcc:location/dcc:postCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:calibrationLaboratory/dcc:contact/dcc:location/dcc:street</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:calibrationLaboratory/dcc:contact/dcc:location/dcc:streetNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:calibrationLaboratory/dcc:contact/dcc:location/dcc:further/dcc:content</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:respPersons/dcc:respPerson/dcc:person/dcc:name/dcc:content</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:customer/dcc:name/dcc:content</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:customer/dcc:eMail</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:customer/dcc:location/dcc:city</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:customer/dcc:location/dcc:countryCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:customer/dcc:location/dcc:postCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:customer/dcc:location/dcc:street</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:customer/dcc:location/dcc:streetNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:customer/dcc:location/dcc:further/dcc:content[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:statements/dcc:statement[1]/dcc:reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:statements/dcc:statement[1]/dcc:traceable</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:statements/dcc:statement[1]/dcc:valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:statements/dcc:statement[1]/dcc:declaration/dcc:content[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:statements/dcc:statement[1]/dcc:respAuthority/dcc:name/dcc:content[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:statements/dcc:statement[2]/dcc:declaration/dcc:content[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:name/dcc:content[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:name/dcc:content[3]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:usedMethods/dcc:usedMethod[1]/dcc:description/dcc:content</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:measuringEquipments/dcc:measuringEquipment/dcc:name/dcc:content[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:measuringEquipments/dcc:measuringEquipment/dcc:manufacturer/dcc:name/dcc:content</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:measuringEquipments/dcc:measuringEquipment/dcc:model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:measuringEquipments/dcc:measuringEquipment/dcc:identifications/dcc:identification[1]/dcc:value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:measuringEquipments/dcc:measuringEquipment/dcc:identifications/dcc:identification[2]/dcc:value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:measuringEquipments/dcc:measuringEquipment/dcc:description/dcc:content</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:influenceConditions/dcc:influenceCondition/dcc:description/dcc:content[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:influenceConditions/dcc:influenceCondition/dcc:data/dcc:quantity/si:hybrid/si:real/si:value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:influenceConditions/dcc:influenceCondition/dcc:data/dcc:quantity/si:hybrid/si:real/si:unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:influenceConditions/dcc:influenceCondition/dcc:data/dcc:quantity/si:hybrid/si:real/si:expandedUnc/si:uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:usedMethods/dcc:usedMethod[1]/dcc:norm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:results/dcc:result/dcc:data/dcc:list/dcc:quantity[1]/dcc:measurementMetaData/dcc:metaData/dcc:data/dcc:quantity/si:hybrid/si:realListXMLList[2]/si:valueXMLList</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:results/dcc:result/dcc:data/dcc:list/dcc:quantity[2]/si:hybrid/si:realListXMLList[1]/si:expandedUncXMLList/si:uncertaintyXMLList</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:results/dcc:result/dcc:data/dcc:list/dcc:quantity[2]/si:hybrid/si:realListXMLList[1]/si:expandedUncXMLList/si:coverageFactorXMLList</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:results/dcc:result/dcc:data/dcc:list/dcc:quantity[2]/si:hybrid/si:realListXMLList[2]/si:valueXMLList</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:results/dcc:result/dcc:data/dcc:list/dcc:quantity[2]/si:hybrid/si:realListXMLList[2]/si:expandedUncXMLList/si:uncertaintyXMLList</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:results/dcc:result/dcc:data/dcc:list/dcc:quantity[2]/si:hybrid/si:realListXMLList[2]/si:expandedUncXMLList/si:coverageFactorXMLList</t>
   </si>
 </sst>
 </file>
@@ -916,7 +1162,44 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -927,6 +1210,51 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0BCFA805-76BF-4AFE-9513-65BAFBCB25EE}" name="Table13" displayName="Table13" ref="A1:R6" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:R6" xr:uid="{0BCFA805-76BF-4AFE-9513-65BAFBCB25EE}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{7378B2CC-F29E-41D1-9E44-CB13F033ED00}" name="id"/>
+    <tableColumn id="2" xr3:uid="{143B470D-A4E9-44CD-A4A5-F41E327CDC78}" name="refID"/>
+    <tableColumn id="3" xr3:uid="{E716D0AF-CFBE-4987-A1B3-355E26E44BC4}" name="name"/>
+    <tableColumn id="4" xr3:uid="{5A708E13-BA26-40AC-A0E0-AC3B29EF5716}" name="description"/>
+    <tableColumn id="5" xr3:uid="{902EAD39-1780-4DC5-A42D-B2BEFB319EC4}" name="countryCodeISO3166_1"/>
+    <tableColumn id="6" xr3:uid="{7652A258-98BD-42AE-BCD8-97C96C4CDD8C}" name="convention"/>
+    <tableColumn id="7" xr3:uid="{71043BA0-DD12-45DC-A3E5-6FC2F64A8D55}" name="traceable"/>
+    <tableColumn id="8" xr3:uid="{3A28F3D9-4A81-401D-8FAB-72B24E0B7AEE}" name="norm"/>
+    <tableColumn id="9" xr3:uid="{739F67C5-AB08-453B-8A10-F2E4E5B1C29B}" name="reference"/>
+    <tableColumn id="11" xr3:uid="{380C116D-2EE4-4E3A-B8DB-672012BEEA74}" name="declaration"/>
+    <tableColumn id="12" xr3:uid="{C18B989C-F6F3-4F35-992E-76CB36AED37C}" name="valid"/>
+    <tableColumn id="13" xr3:uid="{04D00783-B109-4B43-AE02-982A94BF0249}" name="date"/>
+    <tableColumn id="14" xr3:uid="{2517CD01-DA3D-4C57-A107-D2C01303CEE5}" name="preiod"/>
+    <tableColumn id="15" xr3:uid="{F499AF8B-FB86-4DEC-8B7E-BA22E3D4CFB0}" name="respAuthority"/>
+    <tableColumn id="16" xr3:uid="{BF647581-303A-464D-9ABD-5008EFAE7683}" name="data"/>
+    <tableColumn id="17" xr3:uid="{EC61CAA4-1B7C-4004-802C-285F03F2BBD8}" name="nonSIDefinition"/>
+    <tableColumn id="18" xr3:uid="{1208D186-A881-4909-9BAB-121C3E81E27C}" name="nonSIUnits"/>
+    <tableColumn id="19" xr3:uid="{2CAB26DA-738E-4376-90E1-E46320E15B04}" name="location"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FC044B5-24CB-4140-A183-70424C80E6A8}" name="Table1" displayName="Table1" ref="A1:I6" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:I6" xr:uid="{2FC044B5-24CB-4140-A183-70424C80E6A8}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{9BE8681D-A525-4CE6-BBF0-09C6834C3F35}" name="id"/>
+    <tableColumn id="2" xr3:uid="{D2DFE407-3DE1-4137-B626-2330F6833D7F}" name="Customer ID"/>
+    <tableColumn id="3" xr3:uid="{1191B479-1091-4224-9CB6-07A53474B6D2}" name="equipmentClass"/>
+    <tableColumn id="4" xr3:uid="{C1346B76-CF01-45E2-8493-E6507423C09C}" name="description"/>
+    <tableColumn id="5" xr3:uid="{B817EAD7-F640-43C2-852D-96D653DABBD4}" name="swRef"/>
+    <tableColumn id="6" xr3:uid="{8749E8C7-8DEA-4909-B795-44F80FE51BAD}" name="Manufacturer"/>
+    <tableColumn id="7" xr3:uid="{D296A60A-4F1F-488F-9312-9417E3EAA61F}" name="Product Name"/>
+    <tableColumn id="8" xr3:uid="{C45BE798-AB6C-48DE-B2C2-5B1FDB333ED8}" name="Product number"/>
+    <tableColumn id="9" xr3:uid="{111BD3A3-C8CE-4455-836A-745437913EA8}" name="Serial number"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1229,7 +1557,7 @@
   <dimension ref="A2:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1237,6 +1565,7 @@
     <col min="1" max="1" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.08984375" customWidth="1"/>
     <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
@@ -1249,6 +1578,9 @@
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
@@ -1429,15 +1761,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5683CA04-207D-4144-92F8-9A8A86CEED7F}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1447,7 +1780,7 @@
     <col min="3" max="3" width="25.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>83</v>
       </c>
@@ -1457,32 +1790,44 @@
       <c r="C1" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="B2" t="s">
         <v>84</v>
       </c>
       <c r="C2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
         <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>88</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -1492,32 +1837,44 @@
       <c r="C5" s="28" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="B6" t="s">
         <v>92</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>94</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="B8" t="s">
         <v>96</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -1527,48 +1884,66 @@
       <c r="C9" s="28" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="B10" t="s">
         <v>101</v>
       </c>
       <c r="C10" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="B11" t="s">
         <v>103</v>
       </c>
       <c r="C11" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="B12" t="s">
         <v>105</v>
       </c>
       <c r="C12" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="B13" t="s">
         <v>107</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="B14" t="s">
         <v>109</v>
       </c>
       <c r="C14" s="28" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -1578,8 +1953,11 @@
       <c r="C15" s="28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -1589,301 +1967,445 @@
       <c r="C16" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="17" spans="2:3">
+      <c r="D16" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
       <c r="B17" t="s">
         <v>117</v>
       </c>
       <c r="C17" s="29" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="18" spans="2:3">
+      <c r="D17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
       <c r="B18" t="s">
         <v>119</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="19" spans="2:3">
+      <c r="D18" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
       <c r="B19" t="s">
         <v>121</v>
       </c>
       <c r="C19" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="20" spans="2:3">
+      <c r="D19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
       <c r="B20" t="s">
         <v>123</v>
       </c>
       <c r="C20" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="21" spans="2:3">
+      <c r="D20" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
       <c r="B21" t="s">
         <v>125</v>
       </c>
       <c r="C21" s="28" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="22" spans="2:3">
+      <c r="D21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
       <c r="B22" t="s">
         <v>127</v>
       </c>
       <c r="C22" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="23" spans="2:3">
+      <c r="D22" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
       <c r="B23" t="s">
         <v>129</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="24" spans="2:3">
+      <c r="D23" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
       <c r="B24" t="s">
         <v>131</v>
       </c>
       <c r="C24" s="29" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="25" spans="2:3">
+      <c r="D24" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
       <c r="B25" t="s">
         <v>133</v>
       </c>
       <c r="C25" s="28" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="26" spans="2:3">
+      <c r="D25" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
       <c r="B26" t="s">
         <v>135</v>
       </c>
       <c r="C26" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="27" spans="2:3">
+      <c r="D26" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
       <c r="B27" t="s">
         <v>137</v>
       </c>
       <c r="C27" s="29" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="28" spans="2:3">
+      <c r="D27" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
       <c r="B28" t="s">
         <v>139</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="29" spans="2:3">
+      <c r="D28" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
       <c r="B29" t="s">
         <v>141</v>
       </c>
       <c r="C29" s="28" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="30" spans="2:3">
+      <c r="D29" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
       <c r="B30" t="s">
         <v>142</v>
       </c>
       <c r="C30" s="28" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="31" spans="2:3">
+      <c r="D30" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
       <c r="B31" t="s">
         <v>144</v>
       </c>
       <c r="C31" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="32" spans="2:3">
+      <c r="D31" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
       <c r="B32" t="s">
         <v>146</v>
       </c>
       <c r="C32" s="28" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="33" spans="2:3">
+      <c r="D32" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
       <c r="B33" t="s">
         <v>148</v>
       </c>
       <c r="C33" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="34" spans="2:3">
+      <c r="D33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
       <c r="B34" t="s">
         <v>150</v>
       </c>
       <c r="C34" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="35" spans="2:3">
+      <c r="D34" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
       <c r="B35" t="s">
         <v>152</v>
       </c>
       <c r="C35" s="28" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="36" spans="2:3">
+      <c r="D35" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
       <c r="B36" t="s">
         <v>154</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="37" spans="2:3">
+      <c r="D36" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
       <c r="B37" t="s">
         <v>155</v>
       </c>
       <c r="C37" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="38" spans="2:3">
+      <c r="D37" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
       <c r="B38" t="s">
         <v>157</v>
       </c>
       <c r="C38" s="28" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="39" spans="2:3">
+      <c r="D38" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
       <c r="B39" t="s">
         <v>159</v>
       </c>
       <c r="C39" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="40" spans="2:3">
+      <c r="D39" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
       <c r="B40" t="s">
         <v>161</v>
       </c>
       <c r="C40" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="41" spans="2:3">
+      <c r="D40" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
       <c r="B41" t="s">
         <v>163</v>
       </c>
       <c r="C41" s="28" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="42" spans="2:3">
+      <c r="D41" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
       <c r="B42" t="s">
         <v>165</v>
       </c>
       <c r="C42" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="43" spans="2:3">
+      <c r="D42" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
       <c r="B43" t="s">
         <v>167</v>
       </c>
       <c r="C43" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="44" spans="2:3">
+      <c r="D43" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
       <c r="B44" t="s">
         <v>169</v>
       </c>
       <c r="C44" s="28" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="45" spans="2:3">
+      <c r="D44" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
       <c r="B45" t="s">
         <v>171</v>
       </c>
       <c r="C45" s="28" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="46" spans="2:3">
+      <c r="D45" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4">
       <c r="B46" t="s">
         <v>173</v>
       </c>
       <c r="C46" s="28" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="47" spans="2:3">
+      <c r="D46" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
       <c r="B47" t="s">
         <v>175</v>
       </c>
       <c r="C47" s="28" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="48" spans="2:3">
+      <c r="D47" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
       <c r="B48" t="s">
         <v>177</v>
       </c>
       <c r="C48" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="49" spans="2:3">
+      <c r="D48" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
       <c r="B49" t="s">
         <v>179</v>
       </c>
       <c r="C49" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="50" spans="2:3">
+      <c r="D49" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
       <c r="B50" t="s">
         <v>181</v>
       </c>
       <c r="C50" s="28" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="51" spans="2:3">
+      <c r="D50" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
       <c r="B51" t="s">
         <v>183</v>
       </c>
       <c r="C51" s="28" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="52" spans="2:3">
+      <c r="D51" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
       <c r="B52" t="s">
         <v>185</v>
       </c>
       <c r="C52" s="28" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="53" spans="2:3">
+      <c r="D52" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
       <c r="B53" t="s">
         <v>187</v>
       </c>
       <c r="C53" t="s">
         <v>188</v>
+      </c>
+      <c r="D53" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="D54" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="D55" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="D56" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="D57" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4">
+      <c r="D58" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4">
+      <c r="D59" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -1899,25 +2421,155 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C531791-9242-4867-B027-97236DF4A138}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="S1" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181308C0-D531-4746-B510-8FF554CEB31C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="13.26953125" customWidth="1"/>
+    <col min="3" max="3" width="24.7265625" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="24.7265625" customWidth="1"/>
+    <col min="8" max="8" width="16.54296875" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="J1" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updates to the Definitions
</commit_message>
<xml_diff>
--- a/DCC-Table_example3.xlsx
+++ b/DCC-Table_example3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\1901 NY-INFRA-FOT\DCC\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74C6897-BF0F-4B50-A1C9-87EC36332A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A8B2E6-7B52-4A0E-B6AA-1E9F050425BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="1725" windowWidth="25560" windowHeight="14775" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27645" windowHeight="18240" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="473">
   <si>
     <t>customerTag</t>
   </si>
@@ -1276,6 +1276,195 @@
   </si>
   <si>
     <t>Source.Weight</t>
+  </si>
+  <si>
+    <t>\metre</t>
+  </si>
+  <si>
+    <t>\kilogram</t>
+  </si>
+  <si>
+    <t>\second</t>
+  </si>
+  <si>
+    <t>\ampere</t>
+  </si>
+  <si>
+    <t>\mole</t>
+  </si>
+  <si>
+    <t>\candela</t>
+  </si>
+  <si>
+    <t>\one</t>
+  </si>
+  <si>
+    <t>\day</t>
+  </si>
+  <si>
+    <t>\hour</t>
+  </si>
+  <si>
+    <t>\minute</t>
+  </si>
+  <si>
+    <t>\degree</t>
+  </si>
+  <si>
+    <t>\arcminute</t>
+  </si>
+  <si>
+    <t>\arcsecond</t>
+  </si>
+  <si>
+    <t>\gram</t>
+  </si>
+  <si>
+    <t>\radian</t>
+  </si>
+  <si>
+    <t>\steradian</t>
+  </si>
+  <si>
+    <t>\hertz</t>
+  </si>
+  <si>
+    <t>\newton</t>
+  </si>
+  <si>
+    <t>\pascal</t>
+  </si>
+  <si>
+    <t>\joule</t>
+  </si>
+  <si>
+    <t>\watt</t>
+  </si>
+  <si>
+    <t>\coulomb</t>
+  </si>
+  <si>
+    <t>\volt</t>
+  </si>
+  <si>
+    <t>\farad</t>
+  </si>
+  <si>
+    <t>\siemens</t>
+  </si>
+  <si>
+    <t>\weber</t>
+  </si>
+  <si>
+    <t>\tesla</t>
+  </si>
+  <si>
+    <t>\henry</t>
+  </si>
+  <si>
+    <t>\lumen</t>
+  </si>
+  <si>
+    <t>\lux</t>
+  </si>
+  <si>
+    <t>\becquerel</t>
+  </si>
+  <si>
+    <t>\sievert</t>
+  </si>
+  <si>
+    <t>\gray</t>
+  </si>
+  <si>
+    <t>\katal</t>
+  </si>
+  <si>
+    <t>\hectare</t>
+  </si>
+  <si>
+    <t>\litre</t>
+  </si>
+  <si>
+    <t>\tonne</t>
+  </si>
+  <si>
+    <t>\electronvolt</t>
+  </si>
+  <si>
+    <t>\dalton</t>
+  </si>
+  <si>
+    <t>\astronomicalunit</t>
+  </si>
+  <si>
+    <t>\neper</t>
+  </si>
+  <si>
+    <t>\bel</t>
+  </si>
+  <si>
+    <t>\decibel</t>
+  </si>
+  <si>
+    <t>\deca</t>
+  </si>
+  <si>
+    <t>\hecto</t>
+  </si>
+  <si>
+    <t>\kilo</t>
+  </si>
+  <si>
+    <t>\mega</t>
+  </si>
+  <si>
+    <t>\giga</t>
+  </si>
+  <si>
+    <t>\tera</t>
+  </si>
+  <si>
+    <t>\peta</t>
+  </si>
+  <si>
+    <t>\exa</t>
+  </si>
+  <si>
+    <t>\zetta</t>
+  </si>
+  <si>
+    <t>\yotta</t>
+  </si>
+  <si>
+    <t>\deci</t>
+  </si>
+  <si>
+    <t>\centi</t>
+  </si>
+  <si>
+    <t>\milli</t>
+  </si>
+  <si>
+    <t>\micro</t>
+  </si>
+  <si>
+    <t>\nano</t>
+  </si>
+  <si>
+    <t>\pico</t>
+  </si>
+  <si>
+    <t>\femto</t>
+  </si>
+  <si>
+    <t>\atto</t>
+  </si>
+  <si>
+    <t>\zepto</t>
+  </si>
+  <si>
+    <t>\yocto</t>
   </si>
 </sst>
 </file>
@@ -2010,15 +2199,15 @@
   <dimension ref="A1:L152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2032,6 +2221,9 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2045,6 +2237,9 @@
       <c r="C2" s="31" t="s">
         <v>278</v>
       </c>
+      <c r="D2" t="s">
+        <v>410</v>
+      </c>
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12">
@@ -2057,6 +2252,9 @@
       <c r="C3" s="31" t="s">
         <v>279</v>
       </c>
+      <c r="D3" t="s">
+        <v>411</v>
+      </c>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12">
@@ -2069,6 +2267,9 @@
       <c r="C4" s="31" t="s">
         <v>280</v>
       </c>
+      <c r="D4" t="s">
+        <v>412</v>
+      </c>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12">
@@ -2081,6 +2282,9 @@
       <c r="C5" s="31" t="s">
         <v>281</v>
       </c>
+      <c r="D5" t="s">
+        <v>413</v>
+      </c>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
@@ -2089,6 +2293,9 @@
       </c>
       <c r="C6" s="31" t="s">
         <v>282</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
       </c>
       <c r="L6" s="2"/>
     </row>
@@ -2100,6 +2307,9 @@
       <c r="C7" s="31" t="s">
         <v>283</v>
       </c>
+      <c r="D7" t="s">
+        <v>414</v>
+      </c>
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12">
@@ -2109,6 +2319,9 @@
       <c r="C8" s="31" t="s">
         <v>284</v>
       </c>
+      <c r="D8" t="s">
+        <v>415</v>
+      </c>
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12">
@@ -2118,6 +2331,9 @@
       <c r="C9" s="31" t="s">
         <v>285</v>
       </c>
+      <c r="D9" t="s">
+        <v>416</v>
+      </c>
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12">
@@ -2127,6 +2343,9 @@
       <c r="C10" s="31" t="s">
         <v>286</v>
       </c>
+      <c r="D10" t="s">
+        <v>417</v>
+      </c>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12">
@@ -2136,6 +2355,9 @@
       <c r="C11" s="31" t="s">
         <v>287</v>
       </c>
+      <c r="D11" t="s">
+        <v>418</v>
+      </c>
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12">
@@ -2145,6 +2367,9 @@
       <c r="C12" s="31" t="s">
         <v>288</v>
       </c>
+      <c r="D12" t="s">
+        <v>419</v>
+      </c>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12">
@@ -2154,6 +2379,9 @@
       <c r="C13" s="31" t="s">
         <v>289</v>
       </c>
+      <c r="D13" t="s">
+        <v>420</v>
+      </c>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12">
@@ -2163,6 +2391,9 @@
       <c r="C14" s="31" t="s">
         <v>290</v>
       </c>
+      <c r="D14" t="s">
+        <v>421</v>
+      </c>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12">
@@ -2172,6 +2403,9 @@
       <c r="C15" s="31" t="s">
         <v>291</v>
       </c>
+      <c r="D15" t="s">
+        <v>422</v>
+      </c>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12">
@@ -2181,333 +2415,489 @@
       <c r="C16" s="31" t="s">
         <v>292</v>
       </c>
+      <c r="D16" t="s">
+        <v>423</v>
+      </c>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:4">
       <c r="B17" t="s">
         <v>71</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="18" spans="2:3">
+      <c r="D17" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
       <c r="B18" t="s">
         <v>72</v>
       </c>
       <c r="C18" s="31" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="19" spans="2:3">
+      <c r="D18" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
       <c r="B19" t="s">
         <v>75</v>
       </c>
       <c r="C19" s="31" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="20" spans="2:3">
+      <c r="D19" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
       <c r="C20" s="31" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="21" spans="2:3">
+      <c r="D20" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
       <c r="C21" s="31" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="22" spans="2:3">
+      <c r="D21" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
       <c r="C22" s="31" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="23" spans="2:3">
+      <c r="D22" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
       <c r="C23" s="31" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="24" spans="2:3">
+      <c r="D23" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
       <c r="C24" s="31" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="25" spans="2:3">
+      <c r="D24" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
       <c r="C25" s="31" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="26" spans="2:3">
+      <c r="D25" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
       <c r="C26" s="31" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="27" spans="2:3">
+      <c r="D26" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
       <c r="C27" s="31" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="28" spans="2:3">
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
       <c r="C28" s="31" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="29" spans="2:3">
+      <c r="D28" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
       <c r="C29" s="31" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="30" spans="2:3">
+      <c r="D29" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
       <c r="C30" s="31" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="31" spans="2:3">
+      <c r="D30" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
       <c r="C31" s="31" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="32" spans="2:3">
+      <c r="D31" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
       <c r="C32" s="31" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="33" spans="3:3">
+      <c r="D32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4">
       <c r="C33" s="31" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="34" spans="3:3">
+      <c r="D33" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4">
       <c r="C34" s="31" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="35" spans="3:3">
+      <c r="D34" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4">
       <c r="C35" s="31" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="36" spans="3:3">
+      <c r="D35" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4">
       <c r="C36" s="31" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="37" spans="3:3">
+      <c r="D36" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4">
       <c r="C37" s="31" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="38" spans="3:3">
+      <c r="D37" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4">
       <c r="C38" s="31" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="39" spans="3:3">
+      <c r="D38" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4">
       <c r="C39" s="31" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="40" spans="3:3">
+      <c r="D39" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4">
       <c r="C40" s="31" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="41" spans="3:3">
+      <c r="D40" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4">
       <c r="C41" s="31" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="42" spans="3:3">
+      <c r="D41" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4">
       <c r="C42" s="31" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="43" spans="3:3">
+      <c r="D42" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4">
       <c r="C43" s="31" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="44" spans="3:3">
+      <c r="D43" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4">
       <c r="C44" s="31" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="45" spans="3:3">
+      <c r="D44" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4">
       <c r="C45" s="31" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="46" spans="3:3">
+      <c r="D45" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4">
       <c r="C46" s="31" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="47" spans="3:3">
+      <c r="D46" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4">
       <c r="C47" s="31" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="48" spans="3:3">
+      <c r="D47" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4">
       <c r="C48" s="31" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="49" spans="3:3">
+      <c r="D48" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4">
       <c r="C49" s="31" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="50" spans="3:3">
+      <c r="D49" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4">
       <c r="C50" s="31" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="51" spans="3:3">
+      <c r="D50" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4">
       <c r="C51" s="31" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="52" spans="3:3">
+      <c r="D51" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4">
       <c r="C52" s="31" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="53" spans="3:3">
+      <c r="D52" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4">
       <c r="C53" s="31" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="54" spans="3:3">
+      <c r="D53" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4">
       <c r="C54" s="31" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="55" spans="3:3">
+      <c r="D54" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4">
       <c r="C55" s="31" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="56" spans="3:3">
+      <c r="D55" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4">
       <c r="C56" s="31" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="57" spans="3:3">
+      <c r="D56" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4">
       <c r="C57" s="31" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="58" spans="3:3">
+      <c r="D57" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4">
       <c r="C58" s="31" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="59" spans="3:3">
+      <c r="D58" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4">
       <c r="C59" s="31" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="60" spans="3:3">
+      <c r="D59" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4">
       <c r="C60" s="31" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="61" spans="3:3">
+      <c r="D60" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4">
       <c r="C61" s="31" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="62" spans="3:3">
+      <c r="D61" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4">
       <c r="C62" s="31" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="63" spans="3:3">
+      <c r="D62" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4">
       <c r="C63" s="31" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="64" spans="3:3">
+      <c r="D63" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4">
       <c r="C64" s="31" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="65" spans="3:3">
+      <c r="D64" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4">
       <c r="C65" s="31" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="66" spans="3:3">
+      <c r="D65" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4">
       <c r="C66" s="31" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="67" spans="3:3">
+      <c r="D66" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4">
       <c r="C67" s="31" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="68" spans="3:3">
+      <c r="D67" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4">
       <c r="C68" s="31" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="69" spans="3:3">
+    <row r="69" spans="3:4">
       <c r="C69" s="31" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="70" spans="3:3">
+    <row r="70" spans="3:4">
       <c r="C70" s="31" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="71" spans="3:3">
+    <row r="71" spans="3:4">
       <c r="C71" s="31" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="72" spans="3:3">
+    <row r="72" spans="3:4">
       <c r="C72" s="31" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="73" spans="3:3">
+    <row r="73" spans="3:4">
       <c r="C73" s="31" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="74" spans="3:3">
+    <row r="74" spans="3:4">
       <c r="C74" s="31" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="75" spans="3:3">
+    <row r="75" spans="3:4">
       <c r="C75" s="31" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="76" spans="3:3">
+    <row r="76" spans="3:4">
       <c r="C76" s="31" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="77" spans="3:3">
+    <row r="77" spans="3:4">
       <c r="C77" s="31" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="78" spans="3:3">
+    <row r="78" spans="3:4">
       <c r="C78" s="31" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="79" spans="3:3">
+    <row r="79" spans="3:4">
       <c r="C79" s="31" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="80" spans="3:3">
+    <row r="80" spans="3:4">
       <c r="C80" s="31" t="s">
         <v>356</v>
       </c>
@@ -3020,11 +3410,11 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.36328125" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3674,16 +4064,16 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.81640625" customWidth="1"/>
-    <col min="8" max="8" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3729,26 +4119,26 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -3825,16 +4215,16 @@
       <selection sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="24.7265625" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" customWidth="1"/>
-    <col min="7" max="7" width="24.7265625" customWidth="1"/>
-    <col min="8" max="8" width="16.54296875" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3880,24 +4270,24 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.54296875" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="14.54296875" customWidth="1"/>
-    <col min="11" max="11" width="13.7265625" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="12.81640625" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -3980,7 +4370,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="22">
+    <row r="7" spans="1:13" ht="23.25">
       <c r="A7" s="1" t="s">
         <v>78</v>
       </c>
@@ -4021,7 +4411,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="22">
+    <row r="8" spans="1:13" ht="23.25">
       <c r="A8" s="1" t="s">
         <v>77</v>
       </c>
@@ -4062,7 +4452,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" ht="23.25">
       <c r="A9" s="10" t="s">
         <v>61</v>
       </c>
@@ -4099,7 +4489,7 @@
       </c>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" ht="32.5">
+    <row r="10" spans="1:13" ht="45.75">
       <c r="A10" s="11" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
added import in dcctable2xml.py
from pydcc_tables import DccTableColumn, DccTabel
</commit_message>
<xml_diff>
--- a/DCC-Table_example3.xlsx
+++ b/DCC-Table_example3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\1901 NY-INFRA-FOT\DCC\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A8B2E6-7B52-4A0E-B6AA-1E9F050425BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EA8871-677C-4928-B257-C0E34C3EFA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27645" windowHeight="18240" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="37220" windowHeight="21820" activeTab="5" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -2198,16 +2198,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F9C957-7C4E-4161-9FBF-0EC69D9D67E3}">
   <dimension ref="A1:L152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3410,11 +3410,11 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4064,16 +4064,16 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.81640625" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4119,26 +4119,26 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -4215,16 +4215,16 @@
       <selection sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" customWidth="1"/>
+    <col min="3" max="3" width="24.7265625" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="24.7265625" customWidth="1"/>
+    <col min="8" max="8" width="16.54296875" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4269,25 +4269,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C24526-8286-4257-8B46-E195D4F721E3}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.54296875" customWidth="1"/>
+    <col min="11" max="11" width="13.7265625" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -4370,7 +4370,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="23.25">
+    <row r="7" spans="1:13" ht="22">
       <c r="A7" s="1" t="s">
         <v>78</v>
       </c>
@@ -4411,7 +4411,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="23.25">
+    <row r="8" spans="1:13" ht="22">
       <c r="A8" s="1" t="s">
         <v>77</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="23.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="10" t="s">
         <v>61</v>
       </c>
@@ -4489,7 +4489,7 @@
       </c>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" ht="45.75">
+    <row r="10" spans="1:13" ht="32.5">
       <c r="A10" s="11" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Ryddet op i filerne.
mappingLookup.py: fungerer på mass_certificate men ikke på certificate2.xml
</commit_message>
<xml_diff>
--- a/DCC-Table_example3.xlsx
+++ b/DCC-Table_example3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\1901 NY-INFRA-FOT\DCC\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF7BC6D-FC7C-4AB1-B735-11944DE62F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8046EF98-2236-48A4-B2E7-73AA8DEC8196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27645" windowHeight="16440" activeTab="5" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="474">
   <si>
     <t>customerTag</t>
   </si>
@@ -1465,6 +1465,9 @@
   </si>
   <si>
     <t>\yocto</t>
+  </si>
+  <si>
+    <t>nan</t>
   </si>
 </sst>
 </file>
@@ -2202,12 +2205,12 @@
       <selection sqref="A1:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.90625" customWidth="1"/>
-    <col min="2" max="2" width="32.6328125" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3410,11 +3413,11 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4064,16 +4067,16 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.81640625" customWidth="1"/>
-    <col min="8" max="8" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4119,26 +4122,26 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -4215,16 +4218,16 @@
       <selection sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="24.7265625" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" customWidth="1"/>
-    <col min="7" max="7" width="24.7265625" customWidth="1"/>
-    <col min="8" max="8" width="16.54296875" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4270,24 +4273,24 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.54296875" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="14.54296875" customWidth="1"/>
-    <col min="11" max="11" width="13.7265625" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="12.81640625" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -4370,7 +4373,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="22">
+    <row r="7" spans="1:13" ht="23.25">
       <c r="A7" s="1" t="s">
         <v>78</v>
       </c>
@@ -4411,7 +4414,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="22">
+    <row r="8" spans="1:13" ht="23.25">
       <c r="A8" s="1" t="s">
         <v>77</v>
       </c>
@@ -4452,11 +4455,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" ht="23.25">
       <c r="A9" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="14"/>
+      <c r="B9" s="14" t="s">
+        <v>473</v>
+      </c>
       <c r="C9" s="15" t="s">
         <v>22</v>
       </c>
@@ -4487,9 +4492,11 @@
       <c r="L9" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="M9" s="15"/>
-    </row>
-    <row r="10" spans="1:13" ht="32.5">
+      <c r="M9" s="15" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="45.75">
       <c r="A10" s="11" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
validate.py moved into DCCHelpFunctions
</commit_message>
<xml_diff>
--- a/DCC-Table_example3.xlsx
+++ b/DCC-Table_example3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\1901 NY-INFRA-FOT\DCC\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8046EF98-2236-48A4-B2E7-73AA8DEC8196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0393DC-2A03-4196-B008-F45682213DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27645" windowHeight="16440" activeTab="5" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="475">
   <si>
     <t>customerTag</t>
   </si>
@@ -234,12 +234,6 @@
     <t>unit</t>
   </si>
   <si>
-    <t>NN_temperature1</t>
-  </si>
-  <si>
-    <t>item_ID1</t>
-  </si>
-  <si>
     <t>data_row1</t>
   </si>
   <si>
@@ -1468,6 +1462,15 @@
   </si>
   <si>
     <t>nan</t>
+  </si>
+  <si>
+    <t>Customer Tags</t>
+  </si>
+  <si>
+    <t>itemID1</t>
+  </si>
+  <si>
+    <t>TempCal</t>
   </si>
 </sst>
 </file>
@@ -2215,10 +2218,10 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -2227,7 +2230,7 @@
         <v>61</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2238,10 +2241,10 @@
         <v>46</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="L2" s="2"/>
     </row>
@@ -2253,10 +2256,10 @@
         <v>42</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="L3" s="2"/>
     </row>
@@ -2268,10 +2271,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="L4" s="2"/>
     </row>
@@ -2283,10 +2286,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="L5" s="2"/>
     </row>
@@ -2295,7 +2298,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
@@ -2308,10 +2311,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D7" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="L7" s="2"/>
     </row>
@@ -2320,10 +2323,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="L8" s="2"/>
     </row>
@@ -2332,10 +2335,10 @@
         <v>43</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D9" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="L9" s="2"/>
     </row>
@@ -2344,10 +2347,10 @@
         <v>44</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D10" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="L10" s="2"/>
     </row>
@@ -2356,10 +2359,10 @@
         <v>45</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D11" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -2368,10 +2371,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D12" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="L12" s="2"/>
     </row>
@@ -2380,10 +2383,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D13" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="L13" s="2"/>
     </row>
@@ -2392,10 +2395,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D14" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="L14" s="2"/>
     </row>
@@ -2404,10 +2407,10 @@
         <v>36</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D15" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="L15" s="2"/>
     </row>
@@ -2416,105 +2419,105 @@
         <v>41</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D16" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D17" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D18" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D19" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="C20" s="31" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D20" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="C21" s="31" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D21" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="C22" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D22" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="C23" s="31" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D23" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="C24" s="31" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D24" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="C25" s="31" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D25" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="C26" s="31" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D26" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="C27" s="31" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D27" t="s">
         <v>55</v>
@@ -2522,39 +2525,39 @@
     </row>
     <row r="28" spans="2:4">
       <c r="C28" s="31" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D28" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="C29" s="31" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D29" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="C30" s="31" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D30" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="C31" s="31" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D31" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="C32" s="31" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D32" t="s">
         <v>53</v>
@@ -2562,612 +2565,612 @@
     </row>
     <row r="33" spans="3:4">
       <c r="C33" s="31" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D33" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="34" spans="3:4">
       <c r="C34" s="31" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D34" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="35" spans="3:4">
       <c r="C35" s="31" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D35" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="36" spans="3:4">
       <c r="C36" s="31" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D36" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" s="31" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D37" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="38" spans="3:4">
       <c r="C38" s="31" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D38" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="39" spans="3:4">
       <c r="C39" s="31" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D39" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="31" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D40" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="31" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D41" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="42" spans="3:4">
       <c r="C42" s="31" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D42" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="43" spans="3:4">
       <c r="C43" s="31" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D43" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="44" spans="3:4">
       <c r="C44" s="31" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D44" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="45" spans="3:4">
       <c r="C45" s="31" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D45" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="46" spans="3:4">
       <c r="C46" s="31" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D46" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="47" spans="3:4">
       <c r="C47" s="31" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D47" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="48" spans="3:4">
       <c r="C48" s="31" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D48" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="31" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D49" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" s="31" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D50" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="C51" s="31" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D51" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="C52" s="31" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D52" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="53" spans="3:4">
       <c r="C53" s="31" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D53" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="54" spans="3:4">
       <c r="C54" s="31" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D54" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="55" spans="3:4">
       <c r="C55" s="31" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D55" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="56" spans="3:4">
       <c r="C56" s="31" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D56" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="57" spans="3:4">
       <c r="C57" s="31" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D57" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="31" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D58" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" s="31" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D59" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="60" spans="3:4">
       <c r="C60" s="31" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D60" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" s="31" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D61" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="62" spans="3:4">
       <c r="C62" s="31" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D62" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="63" spans="3:4">
       <c r="C63" s="31" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D63" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="64" spans="3:4">
       <c r="C64" s="31" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D64" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" s="31" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D65" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="31" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D66" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" s="31" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D67" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="31" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" s="31" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="31" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="31" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="C72" s="31" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="31" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="C74" s="31" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="C75" s="31" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" s="31" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" s="31" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="31" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="31" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="80" spans="3:4">
       <c r="C80" s="31" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" s="31" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" s="31" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" s="31" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" s="31" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" s="31" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" s="31" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" s="31" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" s="31" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" s="31" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" s="31" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" s="31" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" s="31" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" s="31" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" s="31" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" s="31" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" s="31" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" s="31" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="98" spans="3:3">
       <c r="C98" s="31" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="99" spans="3:3">
       <c r="C99" s="31" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="100" spans="3:3">
       <c r="C100" s="31" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101" s="31" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="102" spans="3:3">
       <c r="C102" s="31" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="103" spans="3:3">
       <c r="C103" s="31" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="104" spans="3:3">
       <c r="C104" s="31" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="105" spans="3:3">
       <c r="C105" s="31" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="106" spans="3:3">
       <c r="C106" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="107" spans="3:3">
       <c r="C107" s="31" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="108" spans="3:3">
       <c r="C108" s="31" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="109" spans="3:3">
       <c r="C109" s="31" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="110" spans="3:3">
       <c r="C110" s="31" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="111" spans="3:3">
       <c r="C111" s="31" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="112" spans="3:3">
       <c r="C112" s="31" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="113" spans="3:3">
       <c r="C113" s="31" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="114" spans="3:3">
       <c r="C114" s="31" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="115" spans="3:3">
       <c r="C115" s="31" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="116" spans="3:3">
       <c r="C116" s="31" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="117" spans="3:3">
       <c r="C117" s="31" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="118" spans="3:3">
       <c r="C118" s="31" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="119" spans="3:3">
       <c r="C119" s="31" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="120" spans="3:3">
       <c r="C120" s="31" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="121" spans="3:3">
       <c r="C121" s="31" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="122" spans="3:3">
       <c r="C122" s="31" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="123" spans="3:3">
       <c r="C123" s="31" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="124" spans="3:3">
       <c r="C124" s="31" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="125" spans="3:3">
       <c r="C125" s="31" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="126" spans="3:3">
       <c r="C126" s="31" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="127" spans="3:3">
       <c r="C127" s="31" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="128" spans="3:3">
       <c r="C128" s="31" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="129" spans="3:3">
       <c r="C129" s="31" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="130" spans="3:3">
       <c r="C130" s="31" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="131" spans="3:3">
       <c r="C131" s="31" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="132" spans="3:3">
       <c r="C132" s="31" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="133" spans="3:3">
       <c r="C133" s="31" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="134" spans="3:3">
@@ -3422,630 +3425,630 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="B9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>100</v>
-      </c>
       <c r="D9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>113</v>
-      </c>
       <c r="D15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s">
         <v>114</v>
       </c>
-      <c r="B16" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" t="s">
-        <v>116</v>
-      </c>
       <c r="D16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D20" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D21" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D22" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D23" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D24" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D26" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D27" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D28" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D29" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D30" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D31" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="B32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D32" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D33" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="B34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D34" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D36" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C37" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D37" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D38" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="39" spans="2:4">
       <c r="B39" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C39" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D39" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C40" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D40" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D41" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C42" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D42" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C43" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="44" spans="2:4">
       <c r="B44" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D44" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="45" spans="2:4">
       <c r="B45" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D45" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D46" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D47" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="B48" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C48" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D48" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="49" spans="2:4">
       <c r="B49" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C49" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D49" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="50" spans="2:4">
       <c r="B50" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D50" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51" spans="2:4">
       <c r="B51" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D51" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D52" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C53" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D53" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="54" spans="2:4">
       <c r="D54" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="55" spans="2:4">
       <c r="D55" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="56" spans="2:4">
       <c r="D56" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="57" spans="2:4">
       <c r="D57" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58" spans="2:4">
       <c r="D58" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="D59" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -4081,28 +4084,28 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>277</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -4146,58 +4149,58 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>39</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>212</v>
       </c>
       <c r="S1" s="3"/>
     </row>
@@ -4232,31 +4235,31 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="J1" s="3"/>
     </row>
@@ -4273,7 +4276,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4303,7 +4306,7 @@
         <v>58</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>62</v>
+        <v>474</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -4311,12 +4314,12 @@
         <v>59</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>63</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" s="27">
         <f>COUNTA(A11:A1048576)</f>
@@ -4325,7 +4328,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B5" s="27">
         <f>COUNTA(B6:XFD6)</f>
@@ -4334,7 +4337,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>34</v>
@@ -4375,7 +4378,7 @@
     </row>
     <row r="7" spans="1:13" ht="23.25">
       <c r="A7" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>0</v>
@@ -4396,10 +4399,10 @@
         <v>46</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>5</v>
@@ -4416,7 +4419,7 @@
     </row>
     <row r="8" spans="1:13" ht="23.25">
       <c r="A8" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>37</v>
@@ -4460,7 +4463,7 @@
         <v>61</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>22</v>
@@ -4493,14 +4496,16 @@
         <v>55</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="45.75">
       <c r="A10" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="14"/>
+      <c r="B10" s="14" t="s">
+        <v>472</v>
+      </c>
       <c r="C10" s="23" t="s">
         <v>33</v>
       </c>
@@ -4517,10 +4522,10 @@
         <v>32</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J10" s="23" t="s">
         <v>47</v>
@@ -4529,15 +4534,15 @@
         <v>50</v>
       </c>
       <c r="L10" s="24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M10" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>27</v>
@@ -4580,7 +4585,7 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>28</v>
@@ -4623,7 +4628,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>29</v>
@@ -4666,7 +4671,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>30</v>
@@ -4709,7 +4714,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
fix unique collumns and accreditationAppliesList
</commit_message>
<xml_diff>
--- a/DCC-Table_example3.xlsx
+++ b/DCC-Table_example3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\1901 NY-INFRA-FOT\DCC\Software\DCCtables\master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\MS\4006-03 AI metrologi\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0393DC-2A03-4196-B008-F45682213DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45B486F-EDFD-4565-A0A1-8999AB6D08AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27645" windowHeight="16440" activeTab="5" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15555" activeTab="5" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -4276,7 +4276,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
update example3 and mass_example
Update excel2table to read in information from the item-sheet of the
workbooks.
</commit_message>
<xml_diff>
--- a/DCC-Table_example3.xlsx
+++ b/DCC-Table_example3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\MS\4006-03 AI metrologi\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45B486F-EDFD-4565-A0A1-8999AB6D08AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DE95D1-A545-4F5A-8E85-548DD073AC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15555" activeTab="5" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
+    <workbookView xWindow="4500" yWindow="525" windowWidth="33855" windowHeight="16515" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="482">
   <si>
     <t>customerTag</t>
   </si>
@@ -222,9 +222,6 @@
     <t>DCCTable</t>
   </si>
   <si>
-    <t>TableID</t>
-  </si>
-  <si>
     <t>refID</t>
   </si>
   <si>
@@ -1471,6 +1468,30 @@
   </si>
   <si>
     <t>TempCal</t>
+  </si>
+  <si>
+    <t>itemID</t>
+  </si>
+  <si>
+    <t>tableID</t>
+  </si>
+  <si>
+    <t>settingID</t>
+  </si>
+  <si>
+    <t>setting01</t>
+  </si>
+  <si>
+    <t>NN32</t>
+  </si>
+  <si>
+    <t>Amitek</t>
+  </si>
+  <si>
+    <t>Platinum Super</t>
+  </si>
+  <si>
+    <t>X34hwk4579</t>
   </si>
 </sst>
 </file>
@@ -2204,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F9C957-7C4E-4161-9FBF-0EC69D9D67E3}">
   <dimension ref="A1:L152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H152" sqref="A1:H152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2218,19 +2239,19 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2241,10 +2262,10 @@
         <v>46</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="L2" s="2"/>
     </row>
@@ -2256,10 +2277,10 @@
         <v>42</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="L3" s="2"/>
     </row>
@@ -2271,10 +2292,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="L4" s="2"/>
     </row>
@@ -2286,10 +2307,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="L5" s="2"/>
     </row>
@@ -2298,7 +2319,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
@@ -2311,10 +2332,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="L7" s="2"/>
     </row>
@@ -2323,10 +2344,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L8" s="2"/>
     </row>
@@ -2335,10 +2356,10 @@
         <v>43</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="L9" s="2"/>
     </row>
@@ -2347,10 +2368,10 @@
         <v>44</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L10" s="2"/>
     </row>
@@ -2359,10 +2380,10 @@
         <v>45</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D11" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -2371,10 +2392,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L12" s="2"/>
     </row>
@@ -2383,10 +2404,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D13" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L13" s="2"/>
     </row>
@@ -2395,10 +2416,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="L14" s="2"/>
     </row>
@@ -2407,10 +2428,10 @@
         <v>36</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D15" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L15" s="2"/>
     </row>
@@ -2419,105 +2440,105 @@
         <v>41</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D17" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D18" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D19" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="C20" s="31" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D20" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="C21" s="31" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D21" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="C22" s="31" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D22" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="C23" s="31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D23" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="C24" s="31" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D24" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="C25" s="31" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D25" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="C26" s="31" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D26" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="C27" s="31" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D27" t="s">
         <v>55</v>
@@ -2525,39 +2546,39 @@
     </row>
     <row r="28" spans="2:4">
       <c r="C28" s="31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D28" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="C29" s="31" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D29" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="C30" s="31" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D30" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="C31" s="31" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D31" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="C32" s="31" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D32" t="s">
         <v>53</v>
@@ -2565,612 +2586,612 @@
     </row>
     <row r="33" spans="3:4">
       <c r="C33" s="31" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D33" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="34" spans="3:4">
       <c r="C34" s="31" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D34" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="35" spans="3:4">
       <c r="C35" s="31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D35" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="36" spans="3:4">
       <c r="C36" s="31" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D36" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" s="31" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D37" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="38" spans="3:4">
       <c r="C38" s="31" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="39" spans="3:4">
       <c r="C39" s="31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D39" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="31" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D40" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="31" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D41" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="42" spans="3:4">
       <c r="C42" s="31" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D42" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="43" spans="3:4">
       <c r="C43" s="31" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D43" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="44" spans="3:4">
       <c r="C44" s="31" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D44" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="45" spans="3:4">
       <c r="C45" s="31" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D45" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="46" spans="3:4">
       <c r="C46" s="31" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D46" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="47" spans="3:4">
       <c r="C47" s="31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D47" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="48" spans="3:4">
       <c r="C48" s="31" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D48" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="31" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D49" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" s="31" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D50" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="C51" s="31" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D51" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="C52" s="31" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D52" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="53" spans="3:4">
       <c r="C53" s="31" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D53" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="54" spans="3:4">
       <c r="C54" s="31" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D54" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="55" spans="3:4">
       <c r="C55" s="31" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D55" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="56" spans="3:4">
       <c r="C56" s="31" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D56" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="57" spans="3:4">
       <c r="C57" s="31" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D57" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="31" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D58" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" s="31" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D59" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="60" spans="3:4">
       <c r="C60" s="31" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D60" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" s="31" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D61" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="62" spans="3:4">
       <c r="C62" s="31" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D62" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="63" spans="3:4">
       <c r="C63" s="31" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D63" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="64" spans="3:4">
       <c r="C64" s="31" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D64" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" s="31" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D65" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D66" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" s="31" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D67" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" s="31" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="31" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="31" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="C72" s="31" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="31" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="C74" s="31" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="C75" s="31" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" s="31" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" s="31" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="31" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="31" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="80" spans="3:4">
       <c r="C80" s="31" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" s="31" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" s="31" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" s="31" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" s="31" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" s="31" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" s="31" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" s="31" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" s="31" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" s="31" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" s="31" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" s="31" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" s="31" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" s="31" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" s="31" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" s="31" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" s="31" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" s="31" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="98" spans="3:3">
       <c r="C98" s="31" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="99" spans="3:3">
       <c r="C99" s="31" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="100" spans="3:3">
       <c r="C100" s="31" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101" s="31" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="102" spans="3:3">
       <c r="C102" s="31" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="103" spans="3:3">
       <c r="C103" s="31" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="104" spans="3:3">
       <c r="C104" s="31" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="105" spans="3:3">
       <c r="C105" s="31" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="106" spans="3:3">
       <c r="C106" s="31" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="107" spans="3:3">
       <c r="C107" s="31" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="108" spans="3:3">
       <c r="C108" s="31" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="109" spans="3:3">
       <c r="C109" s="31" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="110" spans="3:3">
       <c r="C110" s="31" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="111" spans="3:3">
       <c r="C111" s="31" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="112" spans="3:3">
       <c r="C112" s="31" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="113" spans="3:3">
       <c r="C113" s="31" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="114" spans="3:3">
       <c r="C114" s="31" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="115" spans="3:3">
       <c r="C115" s="31" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="116" spans="3:3">
       <c r="C116" s="31" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="117" spans="3:3">
       <c r="C117" s="31" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="118" spans="3:3">
       <c r="C118" s="31" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="119" spans="3:3">
       <c r="C119" s="31" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="120" spans="3:3">
       <c r="C120" s="31" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="121" spans="3:3">
       <c r="C121" s="31" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="122" spans="3:3">
       <c r="C122" s="31" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="123" spans="3:3">
       <c r="C123" s="31" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="124" spans="3:3">
       <c r="C124" s="31" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="125" spans="3:3">
       <c r="C125" s="31" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="126" spans="3:3">
       <c r="C126" s="31" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="127" spans="3:3">
       <c r="C127" s="31" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="128" spans="3:3">
       <c r="C128" s="31" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="129" spans="3:3">
       <c r="C129" s="31" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="130" spans="3:3">
       <c r="C130" s="31" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="131" spans="3:3">
       <c r="C131" s="31" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="132" spans="3:3">
       <c r="C132" s="31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="133" spans="3:3">
       <c r="C133" s="31" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="134" spans="3:3">
@@ -3425,630 +3446,630 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
         <v>82</v>
       </c>
-      <c r="C2" t="s">
-        <v>83</v>
-      </c>
       <c r="D2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
         <v>84</v>
       </c>
-      <c r="C3" t="s">
-        <v>85</v>
-      </c>
       <c r="D3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>87</v>
-      </c>
       <c r="D4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
         <v>88</v>
       </c>
-      <c r="B5" t="s">
-        <v>89</v>
-      </c>
       <c r="C5" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="28" t="s">
-        <v>91</v>
-      </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>93</v>
-      </c>
       <c r="D7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>95</v>
-      </c>
       <c r="D8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="28" t="s">
-        <v>98</v>
-      </c>
       <c r="D9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" t="s">
         <v>99</v>
       </c>
-      <c r="C10" t="s">
-        <v>100</v>
-      </c>
       <c r="D10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" t="s">
         <v>101</v>
       </c>
-      <c r="C11" t="s">
-        <v>102</v>
-      </c>
       <c r="D11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" t="s">
         <v>103</v>
       </c>
-      <c r="C12" t="s">
-        <v>104</v>
-      </c>
       <c r="D12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>106</v>
-      </c>
       <c r="D13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="C14" s="28" t="s">
-        <v>108</v>
-      </c>
       <c r="D14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s">
         <v>109</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="28" t="s">
-        <v>111</v>
-      </c>
       <c r="D15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" t="s">
         <v>112</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>113</v>
       </c>
-      <c r="C16" t="s">
-        <v>114</v>
-      </c>
       <c r="D16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="29" t="s">
-        <v>116</v>
-      </c>
       <c r="D17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="C18" s="28" t="s">
-        <v>118</v>
-      </c>
       <c r="D18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" t="s">
         <v>119</v>
       </c>
-      <c r="C19" t="s">
-        <v>120</v>
-      </c>
       <c r="D19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" t="s">
         <v>121</v>
       </c>
-      <c r="C20" t="s">
-        <v>122</v>
-      </c>
       <c r="D20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="28" t="s">
-        <v>124</v>
-      </c>
       <c r="D21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" t="s">
         <v>125</v>
       </c>
-      <c r="C22" t="s">
-        <v>126</v>
-      </c>
       <c r="D22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="30" t="s">
-        <v>128</v>
-      </c>
       <c r="D23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="29" t="s">
-        <v>130</v>
-      </c>
       <c r="D24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="C25" s="28" t="s">
-        <v>132</v>
-      </c>
       <c r="D25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" t="s">
         <v>133</v>
       </c>
-      <c r="C26" t="s">
-        <v>134</v>
-      </c>
       <c r="D26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="C27" s="29" t="s">
-        <v>136</v>
-      </c>
       <c r="D27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C28" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="28" t="s">
-        <v>138</v>
-      </c>
       <c r="D28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D29" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="C30" s="28" t="s">
-        <v>141</v>
-      </c>
       <c r="D30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" t="s">
         <v>142</v>
       </c>
-      <c r="C31" t="s">
-        <v>143</v>
-      </c>
       <c r="D31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="B32" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="C32" s="28" t="s">
-        <v>145</v>
-      </c>
       <c r="D32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" t="s">
         <v>146</v>
       </c>
-      <c r="C33" t="s">
-        <v>147</v>
-      </c>
       <c r="D33" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="B34" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" t="s">
         <v>148</v>
       </c>
-      <c r="C34" t="s">
-        <v>149</v>
-      </c>
       <c r="D34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="C35" s="28" t="s">
-        <v>151</v>
-      </c>
       <c r="D35" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" t="s">
         <v>153</v>
       </c>
-      <c r="C37" t="s">
-        <v>154</v>
-      </c>
       <c r="D37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" t="s">
+        <v>154</v>
+      </c>
+      <c r="C38" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="C38" s="28" t="s">
-        <v>156</v>
-      </c>
       <c r="D38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="39" spans="2:4">
       <c r="B39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" t="s">
         <v>157</v>
       </c>
-      <c r="C39" t="s">
-        <v>158</v>
-      </c>
       <c r="D39" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" t="s">
         <v>159</v>
       </c>
-      <c r="C40" t="s">
-        <v>160</v>
-      </c>
       <c r="D40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" t="s">
+        <v>160</v>
+      </c>
+      <c r="C41" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="C41" s="28" t="s">
-        <v>162</v>
-      </c>
       <c r="D41" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" t="s">
+        <v>162</v>
+      </c>
+      <c r="C42" t="s">
         <v>163</v>
       </c>
-      <c r="C42" t="s">
-        <v>164</v>
-      </c>
       <c r="D42" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43" t="s">
         <v>165</v>
       </c>
-      <c r="C43" t="s">
-        <v>166</v>
-      </c>
       <c r="D43" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="2:4">
       <c r="B44" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="C44" s="28" t="s">
-        <v>168</v>
-      </c>
       <c r="D44" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="45" spans="2:4">
       <c r="B45" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="C45" s="28" t="s">
-        <v>170</v>
-      </c>
       <c r="D45" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" t="s">
+        <v>170</v>
+      </c>
+      <c r="C46" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="C46" s="28" t="s">
-        <v>172</v>
-      </c>
       <c r="D46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" t="s">
+        <v>172</v>
+      </c>
+      <c r="C47" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="C47" s="28" t="s">
-        <v>174</v>
-      </c>
       <c r="D47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="B48" t="s">
+        <v>174</v>
+      </c>
+      <c r="C48" t="s">
         <v>175</v>
       </c>
-      <c r="C48" t="s">
-        <v>176</v>
-      </c>
       <c r="D48" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="2:4">
       <c r="B49" t="s">
+        <v>176</v>
+      </c>
+      <c r="C49" t="s">
         <v>177</v>
       </c>
-      <c r="C49" t="s">
-        <v>178</v>
-      </c>
       <c r="D49" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="50" spans="2:4">
       <c r="B50" t="s">
+        <v>178</v>
+      </c>
+      <c r="C50" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="C50" s="28" t="s">
-        <v>180</v>
-      </c>
       <c r="D50" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="2:4">
       <c r="B51" t="s">
+        <v>180</v>
+      </c>
+      <c r="C51" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="C51" s="28" t="s">
-        <v>182</v>
-      </c>
       <c r="D51" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" t="s">
+        <v>182</v>
+      </c>
+      <c r="C52" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="C52" s="28" t="s">
-        <v>184</v>
-      </c>
       <c r="D52" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" t="s">
+        <v>184</v>
+      </c>
+      <c r="C53" t="s">
         <v>185</v>
       </c>
-      <c r="C53" t="s">
-        <v>186</v>
-      </c>
       <c r="D53" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="2:4">
       <c r="D54" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="55" spans="2:4">
       <c r="D55" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="56" spans="2:4">
       <c r="D56" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="57" spans="2:4">
       <c r="D57" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="58" spans="2:4">
       <c r="D58" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="D59" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -4084,28 +4105,28 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>274</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>275</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -4149,58 +4170,58 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>39</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="S1" s="3"/>
     </row>
@@ -4215,7 +4236,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181308C0-D531-4746-B510-8FF554CEB31C}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:I6"/>
@@ -4235,33 +4256,62 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>195</v>
-      </c>
       <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B2" t="s">
+        <v>478</v>
+      </c>
+      <c r="C2" t="s">
+        <v>470</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" t="s">
+        <v>470</v>
+      </c>
+      <c r="F2" t="s">
+        <v>479</v>
+      </c>
+      <c r="G2" t="s">
+        <v>480</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>481</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4273,10 +4323,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C24526-8286-4257-8B46-E195D4F721E3}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4284,16 +4334,16 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="14.5703125" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -4303,118 +4353,85 @@
     </row>
     <row r="2" spans="1:13" ht="17.25" customHeight="1">
       <c r="A2" s="27" t="s">
-        <v>58</v>
+        <v>475</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="27" t="s">
-        <v>59</v>
+        <v>474</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="27">
-        <f>COUNTA(A11:A1048576)</f>
-        <v>5</v>
+        <v>476</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" s="27">
-        <f>COUNTA(B6:XFD6)</f>
+        <f>COUNTA(A12:A1048576)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="27">
+        <f>COUNTA(B7:XFD7)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="12" t="s">
+    <row r="7" spans="1:13">
+      <c r="A7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="L7" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M7" s="12" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="23.25">
-      <c r="A7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="23.25">
@@ -4422,190 +4439,188 @@
         <v>75</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="23.25">
+      <c r="A9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="M8" s="12" t="s">
+      <c r="C9" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="M9" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="23.25">
-      <c r="A9" s="10" t="s">
+    <row r="10" spans="1:13" ht="23.25">
+      <c r="A10" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45.75">
+      <c r="A11" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>471</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="M9" s="15" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="45.75">
-      <c r="A10" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>472</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="K10" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="L10" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="M10" s="23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="17" t="s">
+      <c r="B12" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C12" s="18">
         <v>0</v>
       </c>
-      <c r="D11" s="19">
-        <f>ROUND(E11+273.15,2)</f>
+      <c r="D12" s="19">
+        <f>ROUND(E12+273.15,2)</f>
         <v>273.16000000000003</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E12" s="19">
         <v>0.01</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F12" s="9">
         <v>-0.1</v>
       </c>
-      <c r="G11" s="9">
-        <f>ROUND(F11-E11,1)</f>
+      <c r="G12" s="9">
+        <f>ROUND(F12-E12,1)</f>
         <v>-0.1</v>
-      </c>
-      <c r="H11" s="25">
-        <v>0.05</v>
-      </c>
-      <c r="I11" s="26">
-        <v>2</v>
-      </c>
-      <c r="J11" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="L11" s="8">
-        <v>1</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="18">
-        <v>15</v>
-      </c>
-      <c r="D12" s="19">
-        <f t="shared" ref="D12:D15" si="0">ROUND(E12+273.15,2)</f>
-        <v>288.16000000000003</v>
-      </c>
-      <c r="E12" s="19">
-        <v>15.01</v>
-      </c>
-      <c r="F12" s="9">
-        <v>15.1</v>
-      </c>
-      <c r="G12" s="9">
-        <f t="shared" ref="G12:G15" si="1">ROUND(F12-E12,1)</f>
-        <v>0.1</v>
       </c>
       <c r="H12" s="25">
         <v>0.05</v>
@@ -4620,138 +4635,181 @@
         <v>51</v>
       </c>
       <c r="L12" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M12" s="9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="5" t="s">
-        <v>64</v>
+      <c r="A13" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="B13" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="18">
+        <v>15</v>
+      </c>
+      <c r="D13" s="19">
+        <f t="shared" ref="D13:D16" si="0">ROUND(E13+273.15,2)</f>
+        <v>288.16000000000003</v>
+      </c>
+      <c r="E13" s="19">
+        <v>15.01</v>
+      </c>
+      <c r="F13" s="9">
+        <v>15.1</v>
+      </c>
+      <c r="G13" s="9">
+        <f t="shared" ref="G13:G16" si="1">ROUND(F13-E13,1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="I13" s="26">
+        <v>2</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" s="8">
+        <v>2</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C14" s="18">
         <v>25</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D14" s="19">
         <f t="shared" si="0"/>
         <v>298.17</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E14" s="19">
         <v>25.02</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F14" s="9">
         <v>25.2</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G14" s="9">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H14" s="25">
         <v>0.05</v>
       </c>
-      <c r="I13" s="26">
+      <c r="I14" s="26">
         <v>2</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J14" s="9">
         <v>0.2</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K14" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L14" s="8">
         <v>3</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="M14" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="17" t="s">
+    <row r="15" spans="1:13">
+      <c r="A15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C15" s="18">
         <v>15</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D15" s="19">
         <f t="shared" si="0"/>
         <v>288.16000000000003</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E15" s="19">
         <v>15.01</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F15" s="9">
         <v>15.3</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G15" s="9">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H15" s="25">
         <v>0.05</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I15" s="26">
         <v>2</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J15" s="9">
         <v>0.2</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K15" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L15" s="8">
         <v>4</v>
       </c>
-      <c r="M14" s="9" t="s">
+      <c r="M15" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="20" t="s">
+    <row r="16" spans="1:13">
+      <c r="A16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C16" s="21">
         <v>0</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D16" s="19">
         <f t="shared" si="0"/>
         <v>273.16000000000003</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E16" s="22">
         <v>0.01</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F16" s="7">
         <v>0</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G16" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H16" s="25">
         <v>0.05</v>
       </c>
-      <c r="I15" s="26">
+      <c r="I16" s="26">
         <v>2</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J16" s="7">
         <v>0.2</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="K16" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L16" s="4">
         <v>5</v>
       </c>
-      <c r="M15" s="7" t="s">
+      <c r="M16" s="7" t="s">
         <v>48</v>
       </c>
     </row>
@@ -4759,13 +4817,13 @@
   <dataConsolidate/>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:M8" xr:uid="{01692EB9-2CFF-4754-B166-4E8AFE51A7B5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:M9" xr:uid="{01692EB9-2CFF-4754-B166-4E8AFE51A7B5}">
       <formula1>MeasurandType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:M6" xr:uid="{75EA51A4-45EC-43B4-8728-0EBA51E434E4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:M7" xr:uid="{75EA51A4-45EC-43B4-8728-0EBA51E434E4}">
       <formula1>ColType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:M7" xr:uid="{05FBC35F-3A35-49D1-B65B-475EDB16B6B1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:M8" xr:uid="{05FBC35F-3A35-49D1-B65B-475EDB16B6B1}">
       <formula1>MetaType</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
excel2dcc now reads adm data from excell
</commit_message>
<xml_diff>
--- a/DCC-Table_example3.xlsx
+++ b/DCC-Table_example3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\MS\4006-03 AI metrologi\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DE95D1-A545-4F5A-8E85-548DD073AC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9DD19E-47F3-431F-A525-DA0007DE4960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="525" windowWidth="33855" windowHeight="16515" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
+    <workbookView xWindow="6060" yWindow="1575" windowWidth="30705" windowHeight="16065" activeTab="4" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="406">
   <si>
     <t>customerTag</t>
   </si>
@@ -75,21 +75,6 @@
     <t>Other</t>
   </si>
   <si>
-    <t>temperatureAbsolute</t>
-  </si>
-  <si>
-    <t>temperatureDifference</t>
-  </si>
-  <si>
-    <t>pressureInternal</t>
-  </si>
-  <si>
-    <t>pressureAbsolute</t>
-  </si>
-  <si>
-    <t>pressureExcess</t>
-  </si>
-  <si>
     <t>geometryLength</t>
   </si>
   <si>
@@ -312,9 +297,6 @@
     <t>Certificate_no</t>
   </si>
   <si>
-    <t>DFM_CertificateNo</t>
-  </si>
-  <si>
     <t>DFM_OrderNo</t>
   </si>
   <si>
@@ -342,45 +324,9 @@
     <t>2022-02-22</t>
   </si>
   <si>
-    <t>DFM_Item1_Description</t>
-  </si>
-  <si>
-    <t>Digitaltermometer</t>
-  </si>
-  <si>
-    <t>DFM_Item1_Name</t>
-  </si>
-  <si>
-    <t>Fluke</t>
-  </si>
-  <si>
-    <t>DFM_Item1_Maufacturer</t>
-  </si>
-  <si>
     <t>Temperature sensor</t>
   </si>
   <si>
-    <t>DFM_Item1_Model</t>
-  </si>
-  <si>
-    <t>1523</t>
-  </si>
-  <si>
-    <t>DFM_Item1_SerialNo</t>
-  </si>
-  <si>
-    <t>8864333</t>
-  </si>
-  <si>
-    <t>Id_no</t>
-  </si>
-  <si>
-    <t>DFM_Item1_ID</t>
-  </si>
-  <si>
-    <t>DMC-2769</t>
-  </si>
-  <si>
     <t>Supplier_Name</t>
   </si>
   <si>
@@ -423,9 +369,6 @@
     <t>DFM_CalLab_Street1</t>
   </si>
   <si>
-    <t xml:space="preserve">Kogle Alle </t>
-  </si>
-  <si>
     <t>DFM_CalLab_Street_No</t>
   </si>
   <si>
@@ -489,123 +432,6 @@
     <t>Mads Målermand</t>
   </si>
   <si>
-    <t>DFM_Accreditation_CALRegNo</t>
-  </si>
-  <si>
-    <t>DK-255</t>
-  </si>
-  <si>
-    <t>DFM_Accreditation_traceable</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>DFM_Accreditation_valid</t>
-  </si>
-  <si>
-    <t>DFM_Accreditation_Statement</t>
-  </si>
-  <si>
-    <t>The calibration is performed under DANAK accreditation no. 255.\nDANAK is one of the signatories ot the EA Multilateral Agreement and the ILAC multilateral agreement for the mutual recognition of calibration certificates.</t>
-  </si>
-  <si>
-    <t>DFM_Accreditation_Body</t>
-  </si>
-  <si>
-    <t>DANAK</t>
-  </si>
-  <si>
-    <t>DFM_TermsOfUse_Statement</t>
-  </si>
-  <si>
-    <t>This certificate may not be reproduced except in full without the written approval of the laboratory.</t>
-  </si>
-  <si>
-    <t>DFM_Item1_Result1_Name_en</t>
-  </si>
-  <si>
-    <t>Temperatures accordign to ITS-90</t>
-  </si>
-  <si>
-    <t>DFM_Item1_Result1_Name_da</t>
-  </si>
-  <si>
-    <t>Temperaturer i henhold til ITS-90</t>
-  </si>
-  <si>
-    <t>DFM_Procedure</t>
-  </si>
-  <si>
-    <t>DFM proceedure Q2KAL251</t>
-  </si>
-  <si>
-    <t>DFM_Reference1_name</t>
-  </si>
-  <si>
-    <t>Standard Platinum Resistance Thermometer</t>
-  </si>
-  <si>
-    <t>DFM_Reference1_manufacturer</t>
-  </si>
-  <si>
-    <t>Rosemount</t>
-  </si>
-  <si>
-    <t>DFM_Reference1_model</t>
-  </si>
-  <si>
-    <t>162CE</t>
-  </si>
-  <si>
-    <t>DFM_Reference1_serial</t>
-  </si>
-  <si>
-    <t>5091</t>
-  </si>
-  <si>
-    <t>DFM_Reference1_ID</t>
-  </si>
-  <si>
-    <t>DFM-1546</t>
-  </si>
-  <si>
-    <t>DFM_Reference_Statement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature is measured via DFM resistancethermometer Rosemount CE162/5091, with DFM calibration certificate number TIR2015. The calibration is executed in situ. </t>
-  </si>
-  <si>
-    <t>DFM_LabTemperature_Description</t>
-  </si>
-  <si>
-    <t>The calibrations are made at constant temperatures by comparison wiht laboratory standards traceable to SI.</t>
-  </si>
-  <si>
-    <t>DFM_LabTemperature_Value</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>DFM_LabTemperature_Unit</t>
-  </si>
-  <si>
-    <t>\degreeCelcius</t>
-  </si>
-  <si>
-    <t>DFM_LabTemperature_U</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>DFM_Item1_Norm</t>
-  </si>
-  <si>
-    <t>DKD-R 5-1:2018</t>
-  </si>
-  <si>
     <t>Template Label</t>
   </si>
   <si>
@@ -690,12 +516,6 @@
     <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:uniqueIdentifier</t>
   </si>
   <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:identifications/dcc:identification[1]/dcc:value</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:identifications/dcc:identification[2]/dcc:value</t>
-  </si>
-  <si>
     <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:receiptDate</t>
   </si>
   <si>
@@ -705,24 +525,6 @@
     <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:endPerformanceDate</t>
   </si>
   <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:items/dcc:name/dcc:content[1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:items/dcc:item/dcc:name/dcc:content[1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:items/dcc:item/dcc:manufacturer/dcc:name/dcc:content</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:items/dcc:item/dcc:model</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:items/dcc:item/dcc:identifications/dcc:identification[1]/dcc:value</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:items/dcc:item/dcc:identifications/dcc:identification[2]/dcc:value</t>
-  </si>
-  <si>
     <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:calibrationLaboratory/dcc:contact/dcc:name/dcc:content</t>
   </si>
   <si>
@@ -774,87 +576,6 @@
     <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:customer/dcc:location/dcc:streetNo</t>
   </si>
   <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:customer/dcc:location/dcc:further/dcc:content[1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:statements/dcc:statement[1]/dcc:reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:statements/dcc:statement[1]/dcc:traceable</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:statements/dcc:statement[1]/dcc:valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:statements/dcc:statement[1]/dcc:declaration/dcc:content[1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:statements/dcc:statement[1]/dcc:respAuthority/dcc:name/dcc:content[1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:statements/dcc:statement[2]/dcc:declaration/dcc:content[1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:name/dcc:content[2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:name/dcc:content[3]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:usedMethods/dcc:usedMethod[1]/dcc:description/dcc:content</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:measuringEquipments/dcc:measuringEquipment/dcc:name/dcc:content[2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:measuringEquipments/dcc:measuringEquipment/dcc:manufacturer/dcc:name/dcc:content</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:measuringEquipments/dcc:measuringEquipment/dcc:model</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:measuringEquipments/dcc:measuringEquipment/dcc:identifications/dcc:identification[1]/dcc:value</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:measuringEquipments/dcc:measuringEquipment/dcc:identifications/dcc:identification[2]/dcc:value</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:measuringEquipments/dcc:measuringEquipment/dcc:description/dcc:content</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:influenceConditions/dcc:influenceCondition/dcc:description/dcc:content[2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:influenceConditions/dcc:influenceCondition/dcc:data/dcc:quantity/si:hybrid/si:real/si:value</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:influenceConditions/dcc:influenceCondition/dcc:data/dcc:quantity/si:hybrid/si:real/si:unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:influenceConditions/dcc:influenceCondition/dcc:data/dcc:quantity/si:hybrid/si:real/si:expandedUnc/si:uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:usedMethods/dcc:usedMethod[1]/dcc:norm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:results/dcc:result/dcc:data/dcc:list/dcc:quantity[1]/dcc:measurementMetaData/dcc:metaData/dcc:data/dcc:quantity/si:hybrid/si:realListXMLList[2]/si:valueXMLList</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:results/dcc:result/dcc:data/dcc:list/dcc:quantity[2]/si:hybrid/si:realListXMLList[1]/si:expandedUncXMLList/si:uncertaintyXMLList</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:results/dcc:result/dcc:data/dcc:list/dcc:quantity[2]/si:hybrid/si:realListXMLList[1]/si:expandedUncXMLList/si:coverageFactorXMLList</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:results/dcc:result/dcc:data/dcc:list/dcc:quantity[2]/si:hybrid/si:realListXMLList[2]/si:valueXMLList</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:results/dcc:result/dcc:data/dcc:list/dcc:quantity[2]/si:hybrid/si:realListXMLList[2]/si:expandedUncXMLList/si:uncertaintyXMLList</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:measurementResults/dcc:measurementResult/dcc:results/dcc:result/dcc:data/dcc:list/dcc:quantity[2]/si:hybrid/si:realListXMLList[2]/si:expandedUncXMLList/si:coverageFactorXMLList</t>
-  </si>
-  <si>
     <t>swID</t>
   </si>
   <si>
@@ -1492,6 +1213,57 @@
   </si>
   <si>
     <t>X34hwk4579</t>
+  </si>
+  <si>
+    <t>miscelaneous01</t>
+  </si>
+  <si>
+    <t>miscelaneous02</t>
+  </si>
+  <si>
+    <t>miscelaneous03</t>
+  </si>
+  <si>
+    <t>miscelaneous04</t>
+  </si>
+  <si>
+    <t>miscelaneous05</t>
+  </si>
+  <si>
+    <t>statement01</t>
+  </si>
+  <si>
+    <t>Kogle Alle</t>
+  </si>
+  <si>
+    <t>DFM_Customer_Webpage</t>
+  </si>
+  <si>
+    <t>DFM_Customer_Phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:customer/dcc:attPerson</t>
+  </si>
+  <si>
+    <t>Issue Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:issueDate</t>
+  </si>
+  <si>
+    <t>2022-02-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:customerIdentification/dcc:value</t>
+  </si>
+  <si>
+    <t>Performance location</t>
+  </si>
+  <si>
+    <t>laboratory</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:performanceLocation</t>
   </si>
 </sst>
 </file>
@@ -1704,7 +1476,7 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1789,6 +1561,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
@@ -2225,8 +1998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F9C957-7C4E-4161-9FBF-0EC69D9D67E3}">
   <dimension ref="A1:L152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H152" sqref="A1:H152"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2234,83 +2007,84 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>188</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>275</v>
+        <v>182</v>
       </c>
       <c r="D2" t="s">
-        <v>407</v>
+        <v>314</v>
       </c>
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>276</v>
+        <v>183</v>
       </c>
       <c r="D3" t="s">
-        <v>408</v>
+        <v>315</v>
       </c>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>277</v>
+        <v>184</v>
       </c>
       <c r="D4" t="s">
-        <v>409</v>
+        <v>316</v>
       </c>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>278</v>
+        <v>185</v>
       </c>
       <c r="D5" t="s">
-        <v>410</v>
+        <v>317</v>
       </c>
       <c r="L5" s="2"/>
     </row>
@@ -2319,10 +2093,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>279</v>
+        <v>186</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="L6" s="2"/>
     </row>
@@ -2332,10 +2106,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>280</v>
+        <v>187</v>
       </c>
       <c r="D7" t="s">
-        <v>411</v>
+        <v>318</v>
       </c>
       <c r="L7" s="2"/>
     </row>
@@ -2344,46 +2118,46 @@
         <v>6</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>281</v>
+        <v>188</v>
       </c>
       <c r="D8" t="s">
-        <v>412</v>
+        <v>319</v>
       </c>
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12">
       <c r="B9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>282</v>
+        <v>189</v>
       </c>
       <c r="D9" t="s">
-        <v>413</v>
+        <v>320</v>
       </c>
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>283</v>
+        <v>190</v>
       </c>
       <c r="D10" t="s">
-        <v>414</v>
+        <v>321</v>
       </c>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12">
       <c r="B11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>284</v>
+        <v>191</v>
       </c>
       <c r="D11" t="s">
-        <v>415</v>
+        <v>322</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -2392,10 +2166,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>285</v>
+        <v>192</v>
       </c>
       <c r="D12" t="s">
-        <v>416</v>
+        <v>323</v>
       </c>
       <c r="L12" s="2"/>
     </row>
@@ -2404,10 +2178,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>286</v>
+        <v>193</v>
       </c>
       <c r="D13" t="s">
-        <v>417</v>
+        <v>324</v>
       </c>
       <c r="L13" s="2"/>
     </row>
@@ -2416,847 +2190,847 @@
         <v>0</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>287</v>
+        <v>194</v>
       </c>
       <c r="D14" t="s">
-        <v>418</v>
+        <v>325</v>
       </c>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12">
       <c r="B15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>288</v>
+        <v>195</v>
       </c>
       <c r="D15" t="s">
-        <v>419</v>
+        <v>326</v>
       </c>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12">
       <c r="B16" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>289</v>
+        <v>196</v>
       </c>
       <c r="D16" t="s">
-        <v>420</v>
+        <v>327</v>
       </c>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>290</v>
+        <v>197</v>
       </c>
       <c r="D17" t="s">
-        <v>421</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>291</v>
+        <v>198</v>
       </c>
       <c r="D18" t="s">
-        <v>422</v>
+        <v>329</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>292</v>
+        <v>199</v>
       </c>
       <c r="D19" t="s">
-        <v>423</v>
+        <v>330</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="C20" s="31" t="s">
-        <v>293</v>
+        <v>200</v>
       </c>
       <c r="D20" t="s">
-        <v>424</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="C21" s="31" t="s">
-        <v>294</v>
+        <v>201</v>
       </c>
       <c r="D21" t="s">
-        <v>425</v>
+        <v>332</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="C22" s="31" t="s">
-        <v>295</v>
+        <v>202</v>
       </c>
       <c r="D22" t="s">
-        <v>426</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="C23" s="31" t="s">
-        <v>296</v>
+        <v>203</v>
       </c>
       <c r="D23" t="s">
-        <v>427</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="C24" s="31" t="s">
-        <v>297</v>
+        <v>204</v>
       </c>
       <c r="D24" t="s">
-        <v>428</v>
+        <v>335</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="C25" s="31" t="s">
-        <v>298</v>
+        <v>205</v>
       </c>
       <c r="D25" t="s">
-        <v>429</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="C26" s="31" t="s">
-        <v>299</v>
+        <v>206</v>
       </c>
       <c r="D26" t="s">
-        <v>430</v>
+        <v>337</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="C27" s="31" t="s">
-        <v>300</v>
+        <v>207</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="C28" s="31" t="s">
-        <v>301</v>
+        <v>208</v>
       </c>
       <c r="D28" t="s">
-        <v>431</v>
+        <v>338</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="C29" s="31" t="s">
-        <v>302</v>
+        <v>209</v>
       </c>
       <c r="D29" t="s">
-        <v>432</v>
+        <v>339</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="C30" s="31" t="s">
-        <v>303</v>
+        <v>210</v>
       </c>
       <c r="D30" t="s">
-        <v>433</v>
+        <v>340</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="C31" s="31" t="s">
-        <v>304</v>
+        <v>211</v>
       </c>
       <c r="D31" t="s">
-        <v>434</v>
+        <v>341</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="C32" s="31" t="s">
-        <v>305</v>
+        <v>212</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="3:4">
       <c r="C33" s="31" t="s">
-        <v>306</v>
+        <v>213</v>
       </c>
       <c r="D33" t="s">
-        <v>435</v>
+        <v>342</v>
       </c>
     </row>
     <row r="34" spans="3:4">
       <c r="C34" s="31" t="s">
-        <v>307</v>
+        <v>214</v>
       </c>
       <c r="D34" t="s">
-        <v>436</v>
+        <v>343</v>
       </c>
     </row>
     <row r="35" spans="3:4">
       <c r="C35" s="31" t="s">
-        <v>308</v>
+        <v>215</v>
       </c>
       <c r="D35" t="s">
-        <v>437</v>
+        <v>344</v>
       </c>
     </row>
     <row r="36" spans="3:4">
       <c r="C36" s="31" t="s">
-        <v>309</v>
+        <v>216</v>
       </c>
       <c r="D36" t="s">
-        <v>438</v>
+        <v>345</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" s="31" t="s">
-        <v>310</v>
+        <v>217</v>
       </c>
       <c r="D37" t="s">
-        <v>439</v>
+        <v>346</v>
       </c>
     </row>
     <row r="38" spans="3:4">
       <c r="C38" s="31" t="s">
-        <v>311</v>
+        <v>218</v>
       </c>
       <c r="D38" t="s">
-        <v>440</v>
+        <v>347</v>
       </c>
     </row>
     <row r="39" spans="3:4">
       <c r="C39" s="31" t="s">
-        <v>312</v>
+        <v>219</v>
       </c>
       <c r="D39" t="s">
-        <v>441</v>
+        <v>348</v>
       </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="31" t="s">
-        <v>313</v>
+        <v>220</v>
       </c>
       <c r="D40" t="s">
-        <v>442</v>
+        <v>349</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="31" t="s">
-        <v>314</v>
+        <v>221</v>
       </c>
       <c r="D41" t="s">
-        <v>443</v>
+        <v>350</v>
       </c>
     </row>
     <row r="42" spans="3:4">
       <c r="C42" s="31" t="s">
-        <v>315</v>
+        <v>222</v>
       </c>
       <c r="D42" t="s">
-        <v>444</v>
+        <v>351</v>
       </c>
     </row>
     <row r="43" spans="3:4">
       <c r="C43" s="31" t="s">
-        <v>316</v>
+        <v>223</v>
       </c>
       <c r="D43" t="s">
-        <v>445</v>
+        <v>352</v>
       </c>
     </row>
     <row r="44" spans="3:4">
       <c r="C44" s="31" t="s">
-        <v>317</v>
+        <v>224</v>
       </c>
       <c r="D44" t="s">
-        <v>446</v>
+        <v>353</v>
       </c>
     </row>
     <row r="45" spans="3:4">
       <c r="C45" s="31" t="s">
-        <v>318</v>
+        <v>225</v>
       </c>
       <c r="D45" t="s">
-        <v>447</v>
+        <v>354</v>
       </c>
     </row>
     <row r="46" spans="3:4">
       <c r="C46" s="31" t="s">
-        <v>319</v>
+        <v>226</v>
       </c>
       <c r="D46" t="s">
-        <v>448</v>
+        <v>355</v>
       </c>
     </row>
     <row r="47" spans="3:4">
       <c r="C47" s="31" t="s">
-        <v>320</v>
+        <v>227</v>
       </c>
       <c r="D47" t="s">
-        <v>449</v>
+        <v>356</v>
       </c>
     </row>
     <row r="48" spans="3:4">
       <c r="C48" s="31" t="s">
-        <v>321</v>
+        <v>228</v>
       </c>
       <c r="D48" t="s">
-        <v>450</v>
+        <v>357</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="31" t="s">
-        <v>322</v>
+        <v>229</v>
       </c>
       <c r="D49" t="s">
-        <v>451</v>
+        <v>358</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" s="31" t="s">
-        <v>323</v>
+        <v>230</v>
       </c>
       <c r="D50" t="s">
-        <v>452</v>
+        <v>359</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="C51" s="31" t="s">
-        <v>324</v>
+        <v>231</v>
       </c>
       <c r="D51" t="s">
-        <v>453</v>
+        <v>360</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="C52" s="31" t="s">
-        <v>325</v>
+        <v>232</v>
       </c>
       <c r="D52" t="s">
-        <v>454</v>
+        <v>361</v>
       </c>
     </row>
     <row r="53" spans="3:4">
       <c r="C53" s="31" t="s">
-        <v>326</v>
+        <v>233</v>
       </c>
       <c r="D53" t="s">
-        <v>455</v>
+        <v>362</v>
       </c>
     </row>
     <row r="54" spans="3:4">
       <c r="C54" s="31" t="s">
-        <v>327</v>
+        <v>234</v>
       </c>
       <c r="D54" t="s">
-        <v>456</v>
+        <v>363</v>
       </c>
     </row>
     <row r="55" spans="3:4">
       <c r="C55" s="31" t="s">
-        <v>328</v>
+        <v>235</v>
       </c>
       <c r="D55" t="s">
-        <v>457</v>
+        <v>364</v>
       </c>
     </row>
     <row r="56" spans="3:4">
       <c r="C56" s="31" t="s">
-        <v>329</v>
+        <v>236</v>
       </c>
       <c r="D56" t="s">
-        <v>458</v>
+        <v>365</v>
       </c>
     </row>
     <row r="57" spans="3:4">
       <c r="C57" s="31" t="s">
-        <v>330</v>
+        <v>237</v>
       </c>
       <c r="D57" t="s">
-        <v>459</v>
+        <v>366</v>
       </c>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="31" t="s">
-        <v>331</v>
+        <v>238</v>
       </c>
       <c r="D58" t="s">
-        <v>460</v>
+        <v>367</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" s="31" t="s">
-        <v>332</v>
+        <v>239</v>
       </c>
       <c r="D59" t="s">
-        <v>461</v>
+        <v>368</v>
       </c>
     </row>
     <row r="60" spans="3:4">
       <c r="C60" s="31" t="s">
-        <v>333</v>
+        <v>240</v>
       </c>
       <c r="D60" t="s">
-        <v>462</v>
+        <v>369</v>
       </c>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" s="31" t="s">
-        <v>334</v>
+        <v>241</v>
       </c>
       <c r="D61" t="s">
-        <v>463</v>
+        <v>370</v>
       </c>
     </row>
     <row r="62" spans="3:4">
       <c r="C62" s="31" t="s">
-        <v>335</v>
+        <v>242</v>
       </c>
       <c r="D62" t="s">
-        <v>464</v>
+        <v>371</v>
       </c>
     </row>
     <row r="63" spans="3:4">
       <c r="C63" s="31" t="s">
-        <v>336</v>
+        <v>243</v>
       </c>
       <c r="D63" t="s">
-        <v>465</v>
+        <v>372</v>
       </c>
     </row>
     <row r="64" spans="3:4">
       <c r="C64" s="31" t="s">
-        <v>337</v>
+        <v>244</v>
       </c>
       <c r="D64" t="s">
-        <v>466</v>
+        <v>373</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" s="31" t="s">
-        <v>338</v>
+        <v>245</v>
       </c>
       <c r="D65" t="s">
-        <v>467</v>
+        <v>374</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="31" t="s">
-        <v>339</v>
+        <v>246</v>
       </c>
       <c r="D66" t="s">
-        <v>468</v>
+        <v>375</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" s="31" t="s">
-        <v>340</v>
+        <v>247</v>
       </c>
       <c r="D67" t="s">
-        <v>469</v>
+        <v>376</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="31" t="s">
-        <v>341</v>
+        <v>248</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" s="31" t="s">
-        <v>342</v>
+        <v>249</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="31" t="s">
-        <v>343</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="31" t="s">
-        <v>344</v>
+        <v>251</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="C72" s="31" t="s">
-        <v>345</v>
+        <v>252</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="31" t="s">
-        <v>346</v>
+        <v>253</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="C74" s="31" t="s">
-        <v>347</v>
+        <v>254</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="C75" s="31" t="s">
-        <v>348</v>
+        <v>255</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" s="31" t="s">
-        <v>349</v>
+        <v>256</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" s="31" t="s">
-        <v>350</v>
+        <v>257</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="31" t="s">
-        <v>351</v>
+        <v>258</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="31" t="s">
-        <v>352</v>
+        <v>259</v>
       </c>
     </row>
     <row r="80" spans="3:4">
       <c r="C80" s="31" t="s">
-        <v>353</v>
+        <v>260</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" s="31" t="s">
-        <v>354</v>
+        <v>261</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" s="31" t="s">
-        <v>355</v>
+        <v>262</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" s="31" t="s">
-        <v>356</v>
+        <v>263</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" s="31" t="s">
-        <v>357</v>
+        <v>264</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" s="31" t="s">
-        <v>358</v>
+        <v>265</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" s="31" t="s">
-        <v>359</v>
+        <v>266</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" s="31" t="s">
-        <v>360</v>
+        <v>267</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" s="31" t="s">
-        <v>361</v>
+        <v>268</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" s="31" t="s">
-        <v>362</v>
+        <v>269</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" s="31" t="s">
-        <v>363</v>
+        <v>270</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" s="31" t="s">
-        <v>364</v>
+        <v>271</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" s="31" t="s">
-        <v>365</v>
+        <v>272</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" s="31" t="s">
-        <v>366</v>
+        <v>273</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" s="31" t="s">
-        <v>367</v>
+        <v>274</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" s="31" t="s">
-        <v>368</v>
+        <v>275</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" s="31" t="s">
-        <v>369</v>
+        <v>276</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" s="31" t="s">
-        <v>370</v>
+        <v>277</v>
       </c>
     </row>
     <row r="98" spans="3:3">
       <c r="C98" s="31" t="s">
-        <v>371</v>
+        <v>278</v>
       </c>
     </row>
     <row r="99" spans="3:3">
       <c r="C99" s="31" t="s">
-        <v>372</v>
+        <v>279</v>
       </c>
     </row>
     <row r="100" spans="3:3">
       <c r="C100" s="31" t="s">
-        <v>373</v>
+        <v>280</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101" s="31" t="s">
-        <v>374</v>
+        <v>281</v>
       </c>
     </row>
     <row r="102" spans="3:3">
       <c r="C102" s="31" t="s">
-        <v>375</v>
+        <v>282</v>
       </c>
     </row>
     <row r="103" spans="3:3">
       <c r="C103" s="31" t="s">
-        <v>376</v>
+        <v>283</v>
       </c>
     </row>
     <row r="104" spans="3:3">
       <c r="C104" s="31" t="s">
-        <v>377</v>
+        <v>284</v>
       </c>
     </row>
     <row r="105" spans="3:3">
       <c r="C105" s="31" t="s">
-        <v>378</v>
+        <v>285</v>
       </c>
     </row>
     <row r="106" spans="3:3">
       <c r="C106" s="31" t="s">
-        <v>379</v>
+        <v>286</v>
       </c>
     </row>
     <row r="107" spans="3:3">
       <c r="C107" s="31" t="s">
-        <v>380</v>
+        <v>287</v>
       </c>
     </row>
     <row r="108" spans="3:3">
       <c r="C108" s="31" t="s">
-        <v>381</v>
+        <v>288</v>
       </c>
     </row>
     <row r="109" spans="3:3">
       <c r="C109" s="31" t="s">
-        <v>382</v>
+        <v>289</v>
       </c>
     </row>
     <row r="110" spans="3:3">
       <c r="C110" s="31" t="s">
-        <v>383</v>
+        <v>290</v>
       </c>
     </row>
     <row r="111" spans="3:3">
       <c r="C111" s="31" t="s">
-        <v>384</v>
+        <v>291</v>
       </c>
     </row>
     <row r="112" spans="3:3">
       <c r="C112" s="31" t="s">
-        <v>385</v>
+        <v>292</v>
       </c>
     </row>
     <row r="113" spans="3:3">
       <c r="C113" s="31" t="s">
-        <v>386</v>
+        <v>293</v>
       </c>
     </row>
     <row r="114" spans="3:3">
       <c r="C114" s="31" t="s">
-        <v>387</v>
+        <v>294</v>
       </c>
     </row>
     <row r="115" spans="3:3">
       <c r="C115" s="31" t="s">
-        <v>388</v>
+        <v>295</v>
       </c>
     </row>
     <row r="116" spans="3:3">
       <c r="C116" s="31" t="s">
-        <v>389</v>
+        <v>296</v>
       </c>
     </row>
     <row r="117" spans="3:3">
       <c r="C117" s="31" t="s">
-        <v>390</v>
+        <v>297</v>
       </c>
     </row>
     <row r="118" spans="3:3">
       <c r="C118" s="31" t="s">
-        <v>391</v>
+        <v>298</v>
       </c>
     </row>
     <row r="119" spans="3:3">
       <c r="C119" s="31" t="s">
-        <v>392</v>
+        <v>299</v>
       </c>
     </row>
     <row r="120" spans="3:3">
       <c r="C120" s="31" t="s">
-        <v>393</v>
+        <v>300</v>
       </c>
     </row>
     <row r="121" spans="3:3">
       <c r="C121" s="31" t="s">
-        <v>394</v>
+        <v>301</v>
       </c>
     </row>
     <row r="122" spans="3:3">
       <c r="C122" s="31" t="s">
-        <v>395</v>
+        <v>302</v>
       </c>
     </row>
     <row r="123" spans="3:3">
       <c r="C123" s="31" t="s">
-        <v>396</v>
+        <v>303</v>
       </c>
     </row>
     <row r="124" spans="3:3">
       <c r="C124" s="31" t="s">
-        <v>397</v>
+        <v>304</v>
       </c>
     </row>
     <row r="125" spans="3:3">
       <c r="C125" s="31" t="s">
-        <v>398</v>
+        <v>305</v>
       </c>
     </row>
     <row r="126" spans="3:3">
       <c r="C126" s="31" t="s">
-        <v>399</v>
+        <v>306</v>
       </c>
     </row>
     <row r="127" spans="3:3">
       <c r="C127" s="31" t="s">
-        <v>400</v>
+        <v>307</v>
       </c>
     </row>
     <row r="128" spans="3:3">
       <c r="C128" s="31" t="s">
-        <v>401</v>
+        <v>308</v>
       </c>
     </row>
     <row r="129" spans="3:3">
       <c r="C129" s="31" t="s">
-        <v>402</v>
+        <v>309</v>
       </c>
     </row>
     <row r="130" spans="3:3">
       <c r="C130" s="31" t="s">
-        <v>403</v>
+        <v>310</v>
       </c>
     </row>
     <row r="131" spans="3:3">
       <c r="C131" s="31" t="s">
-        <v>404</v>
+        <v>311</v>
       </c>
     </row>
     <row r="132" spans="3:3">
       <c r="C132" s="31" t="s">
-        <v>405</v>
+        <v>312</v>
       </c>
     </row>
     <row r="133" spans="3:3">
       <c r="C133" s="31" t="s">
-        <v>406</v>
+        <v>313</v>
       </c>
     </row>
     <row r="134" spans="3:3">
       <c r="C134" t="s">
-        <v>9</v>
+        <v>389</v>
       </c>
     </row>
     <row r="135" spans="3:3">
       <c r="C135" t="s">
-        <v>10</v>
+        <v>390</v>
       </c>
     </row>
     <row r="136" spans="3:3">
       <c r="C136" t="s">
-        <v>11</v>
+        <v>391</v>
       </c>
     </row>
     <row r="137" spans="3:3">
       <c r="C137" t="s">
-        <v>12</v>
+        <v>392</v>
       </c>
     </row>
     <row r="138" spans="3:3">
       <c r="C138" t="s">
-        <v>13</v>
+        <v>393</v>
       </c>
     </row>
     <row r="139" spans="3:3">
       <c r="C139" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="140" spans="3:3">
       <c r="C140" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141" spans="3:3">
       <c r="C141" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="142" spans="3:3">
       <c r="C142" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="143" spans="3:3">
       <c r="C143" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="144" spans="3:3">
       <c r="C144" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="3:3">
       <c r="C145" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="146" spans="3:3">
       <c r="C146" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="147" spans="3:3">
@@ -3271,25 +3045,26 @@
     </row>
     <row r="149" spans="3:3">
       <c r="C149" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="150" spans="3:3">
       <c r="C150" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="151" spans="3:3">
       <c r="C151" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="152" spans="3:3">
       <c r="C152" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://www.metrology.net/wiki/testprocess-measure-capacitance/" xr:uid="{341EFCF9-8FEE-4938-B3BE-D7AA66027F09}"/>
     <hyperlink ref="C3" r:id="rId2" display="https://www.metrology.net/wiki/testprocess-measure-conductance/" xr:uid="{A1463CA9-ED67-4612-8419-FC125E277657}"/>
@@ -3431,10 +3206,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5683CA04-207D-4144-92F8-9A8A86CEED7F}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3446,638 +3221,375 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>186</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>210</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>211</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
         <v>83</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="B4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>86</v>
-      </c>
       <c r="D5" t="s">
-        <v>214</v>
+        <v>402</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>215</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="B8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>94</v>
-      </c>
       <c r="D8" t="s">
-        <v>217</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>95</v>
-      </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>403</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>97</v>
+        <v>404</v>
       </c>
       <c r="D9" t="s">
-        <v>218</v>
+        <v>405</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" t="s">
-        <v>99</v>
+        <v>399</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>401</v>
       </c>
       <c r="D10" t="s">
-        <v>219</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>93</v>
+      </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>220</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="D12" t="s">
-        <v>221</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D13" t="s">
-        <v>222</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>107</v>
+        <v>100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>101</v>
       </c>
       <c r="D14" t="s">
-        <v>223</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>108</v>
-      </c>
       <c r="B15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>110</v>
+        <v>102</v>
+      </c>
+      <c r="C15" t="s">
+        <v>103</v>
       </c>
       <c r="D15" t="s">
-        <v>224</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>111</v>
-      </c>
       <c r="B16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" t="s">
-        <v>113</v>
+        <v>104</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>105</v>
       </c>
       <c r="D16" t="s">
-        <v>225</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>114</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>115</v>
+        <v>106</v>
+      </c>
+      <c r="C17" t="s">
+        <v>395</v>
       </c>
       <c r="D17" t="s">
-        <v>226</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>116</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>108</v>
       </c>
       <c r="D18" t="s">
-        <v>227</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" t="s">
-        <v>119</v>
+        <v>109</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>110</v>
       </c>
       <c r="D19" t="s">
-        <v>228</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C20" t="s">
-        <v>121</v>
+        <v>111</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>112</v>
       </c>
       <c r="D20" t="s">
-        <v>229</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>123</v>
+        <v>113</v>
+      </c>
+      <c r="C21" t="s">
+        <v>114</v>
       </c>
       <c r="D21" t="s">
-        <v>230</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C22" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D22" t="s">
-        <v>231</v>
+        <v>398</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>126</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>127</v>
+        <v>115</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>116</v>
       </c>
       <c r="D23" t="s">
-        <v>232</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
-        <v>128</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>129</v>
+        <v>117</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>118</v>
       </c>
       <c r="D24" t="s">
-        <v>233</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>130</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="D25" t="s">
-        <v>234</v>
-      </c>
+        <v>397</v>
+      </c>
+      <c r="C25" s="28"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C26" t="s">
-        <v>133</v>
+        <v>119</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>103</v>
       </c>
       <c r="D26" t="s">
-        <v>235</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
-        <v>134</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>135</v>
+        <v>120</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>121</v>
       </c>
       <c r="D27" t="s">
-        <v>236</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
-        <v>136</v>
-      </c>
-      <c r="C28" s="28" t="s">
-        <v>137</v>
+        <v>122</v>
+      </c>
+      <c r="C28" t="s">
+        <v>123</v>
       </c>
       <c r="D28" t="s">
-        <v>237</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D29" t="s">
-        <v>238</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" t="s">
-        <v>139</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="D30" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31" t="s">
-        <v>141</v>
-      </c>
-      <c r="C31" t="s">
-        <v>142</v>
-      </c>
-      <c r="D31" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32" t="s">
-        <v>143</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="D32" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33" t="s">
-        <v>145</v>
-      </c>
-      <c r="C33" t="s">
-        <v>146</v>
-      </c>
-      <c r="D33" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" t="s">
-        <v>147</v>
-      </c>
-      <c r="C34" t="s">
-        <v>148</v>
-      </c>
-      <c r="D34" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4">
-      <c r="B35" t="s">
-        <v>149</v>
-      </c>
-      <c r="C35" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="D35" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4">
-      <c r="B36" t="s">
-        <v>151</v>
-      </c>
-      <c r="C36" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="D36" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4">
-      <c r="B37" t="s">
-        <v>152</v>
-      </c>
-      <c r="C37" t="s">
-        <v>153</v>
-      </c>
-      <c r="D37" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4">
-      <c r="B38" t="s">
-        <v>154</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="D38" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4">
-      <c r="B39" t="s">
-        <v>156</v>
-      </c>
-      <c r="C39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D39" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4">
-      <c r="B40" t="s">
-        <v>158</v>
-      </c>
-      <c r="C40" t="s">
-        <v>159</v>
-      </c>
-      <c r="D40" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4">
-      <c r="B41" t="s">
-        <v>160</v>
-      </c>
-      <c r="C41" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="D41" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4">
-      <c r="B42" t="s">
-        <v>162</v>
-      </c>
-      <c r="C42" t="s">
-        <v>163</v>
-      </c>
-      <c r="D42" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4">
-      <c r="B43" t="s">
-        <v>164</v>
-      </c>
-      <c r="C43" t="s">
-        <v>165</v>
-      </c>
-      <c r="D43" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4">
-      <c r="B44" t="s">
-        <v>166</v>
-      </c>
-      <c r="C44" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="D44" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4">
-      <c r="B45" t="s">
-        <v>168</v>
-      </c>
-      <c r="C45" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="D45" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4">
-      <c r="B46" t="s">
-        <v>170</v>
-      </c>
-      <c r="C46" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="D46" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4">
-      <c r="B47" t="s">
-        <v>172</v>
-      </c>
-      <c r="C47" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="D47" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4">
-      <c r="B48" t="s">
-        <v>174</v>
-      </c>
-      <c r="C48" t="s">
-        <v>175</v>
-      </c>
-      <c r="D48" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4">
-      <c r="B49" t="s">
-        <v>176</v>
-      </c>
-      <c r="C49" t="s">
-        <v>177</v>
-      </c>
-      <c r="D49" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4">
-      <c r="B50" t="s">
-        <v>178</v>
-      </c>
-      <c r="C50" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="D50" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4">
-      <c r="B51" t="s">
-        <v>180</v>
-      </c>
-      <c r="C51" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="D51" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4">
-      <c r="B52" t="s">
-        <v>182</v>
-      </c>
-      <c r="C52" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="D52" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4">
-      <c r="B53" t="s">
-        <v>184</v>
-      </c>
-      <c r="C53" t="s">
-        <v>185</v>
-      </c>
-      <c r="D53" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4">
-      <c r="D54" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4">
-      <c r="D55" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4">
-      <c r="D56" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4">
-      <c r="D57" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4">
-      <c r="D58" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4">
-      <c r="D59" t="s">
-        <v>268</v>
-      </c>
+        <v>396</v>
+      </c>
+      <c r="C30" s="28"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="28"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="28"/>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="28"/>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="28"/>
+    </row>
+    <row r="42" spans="3:3">
+      <c r="C42" s="28"/>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="28"/>
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" s="28"/>
+    </row>
+    <row r="45" spans="3:3">
+      <c r="C45" s="28"/>
+    </row>
+    <row r="48" spans="3:3">
+      <c r="C48" s="28"/>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" s="28"/>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50" s="28"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C23" r:id="rId1" display="www.dfm.dk" xr:uid="{E465C636-D594-413A-8B1A-468AA9848358}"/>
-    <hyperlink ref="C17" r:id="rId2" xr:uid="{924EC528-40C3-4804-BF99-CB9DC88AD4BA}"/>
-    <hyperlink ref="C24" r:id="rId3" xr:uid="{A9AAC80D-9488-47F1-80E3-8644FDD89076}"/>
-    <hyperlink ref="C27" r:id="rId4" xr:uid="{AC76966B-0028-4873-8565-AED87429289E}"/>
+    <hyperlink ref="C18" r:id="rId1" display="www.dfm.dk" xr:uid="{E465C636-D594-413A-8B1A-468AA9848358}"/>
+    <hyperlink ref="C12" r:id="rId2" xr:uid="{924EC528-40C3-4804-BF99-CB9DC88AD4BA}"/>
+    <hyperlink ref="C19" r:id="rId3" xr:uid="{A9AAC80D-9488-47F1-80E3-8644FDD89076}"/>
+    <hyperlink ref="C23" r:id="rId4" xr:uid="{AC76966B-0028-4873-8565-AED87429289E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4105,28 +3617,28 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>269</v>
+        <v>176</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>196</v>
+        <v>138</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>270</v>
+        <v>177</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>271</v>
+        <v>178</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>189</v>
+        <v>131</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>272</v>
+        <v>179</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>273</v>
+        <v>180</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>274</v>
+        <v>181</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -4140,26 +3652,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C531791-9242-4867-B027-97236DF4A138}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" customWidth="1"/>
     <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1"/>
@@ -4170,60 +3682,65 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
-        <v>187</v>
+        <v>129</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>196</v>
+        <v>138</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>189</v>
+        <v>131</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>197</v>
+        <v>139</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>198</v>
+        <v>140</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>199</v>
+        <v>141</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>200</v>
+        <v>142</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>201</v>
+        <v>143</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>202</v>
+        <v>144</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>203</v>
+        <v>145</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>204</v>
+        <v>146</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>205</v>
+        <v>147</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>206</v>
+        <v>148</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>207</v>
+        <v>149</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>208</v>
+        <v>150</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>209</v>
+        <v>151</v>
       </c>
       <c r="S1" s="3"/>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" t="s">
+        <v>394</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -4238,8 +3755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181308C0-D531-4746-B510-8FF554CEB31C}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4256,61 +3773,61 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
-        <v>187</v>
+        <v>129</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>192</v>
+        <v>134</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>188</v>
+        <v>130</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>189</v>
+        <v>131</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>190</v>
+        <v>132</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>191</v>
+        <v>133</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>195</v>
+        <v>137</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>193</v>
+        <v>135</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>194</v>
+        <v>136</v>
       </c>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>472</v>
+        <v>379</v>
       </c>
       <c r="B2" t="s">
-        <v>478</v>
+        <v>385</v>
       </c>
       <c r="C2" t="s">
-        <v>470</v>
+        <v>377</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
-        <v>470</v>
+        <v>377</v>
       </c>
       <c r="F2" t="s">
-        <v>479</v>
+        <v>386</v>
       </c>
       <c r="G2" t="s">
-        <v>480</v>
+        <v>387</v>
       </c>
       <c r="H2">
         <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>481</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -4326,7 +3843,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4348,36 +3865,36 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17.25" customHeight="1">
       <c r="A2" s="27" t="s">
-        <v>475</v>
+        <v>382</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>473</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="27" t="s">
-        <v>474</v>
+        <v>381</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>472</v>
+        <v>379</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="27" t="s">
-        <v>476</v>
+        <v>383</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>477</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="27" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B5" s="27">
         <f>COUNTA(A12:A1048576)</f>
@@ -4386,7 +3903,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="27" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B6" s="27">
         <f>COUNTA(B7:XFD7)</f>
@@ -4395,72 +3912,72 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>39</v>
-      </c>
       <c r="D7" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>40</v>
-      </c>
       <c r="M7" s="12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="23.25">
       <c r="A8" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>5</v>
@@ -4469,141 +3986,141 @@
         <v>6</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="23.25">
       <c r="A9" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>332</v>
+        <v>239</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>332</v>
+        <v>239</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>332</v>
+        <v>239</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>332</v>
+        <v>239</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>332</v>
+        <v>239</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>332</v>
+        <v>239</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>332</v>
+        <v>239</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>332</v>
+        <v>239</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>332</v>
+        <v>239</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>331</v>
+        <v>238</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="23.25">
       <c r="A10" s="10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>470</v>
+        <v>377</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>470</v>
+        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45.75">
       <c r="A11" s="11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>471</v>
+        <v>378</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="I11" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="L11" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="J11" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="K11" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="L11" s="24" t="s">
-        <v>76</v>
-      </c>
       <c r="M11" s="23" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C12" s="18">
         <v>0</v>
@@ -4632,21 +4149,21 @@
         <v>0.2</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="L12" s="8">
         <v>1</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C13" s="18">
         <v>15</v>
@@ -4675,21 +4192,21 @@
         <v>0.2</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="L13" s="8">
         <v>2</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C14" s="18">
         <v>25</v>
@@ -4718,21 +4235,21 @@
         <v>0.2</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="L14" s="8">
         <v>3</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C15" s="18">
         <v>15</v>
@@ -4761,21 +4278,21 @@
         <v>0.2</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="L15" s="8">
         <v>4</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C16" s="21">
         <v>0</v>
@@ -4804,13 +4321,13 @@
         <v>0.2</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="L16" s="4">
         <v>5</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more attributes to table-element
</commit_message>
<xml_diff>
--- a/DCC-Table_example3.xlsx
+++ b/DCC-Table_example3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\MS\4006-03 AI metrologi\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9DD19E-47F3-431F-A525-DA0007DE4960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09607813-8499-453E-942B-3CB7332DBBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="1575" windowWidth="30705" windowHeight="16065" activeTab="4" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
+    <workbookView xWindow="3855" yWindow="2640" windowWidth="33540" windowHeight="12615" activeTab="3" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -20,10 +20,14 @@
     <sheet name="Items" sheetId="7" r:id="rId5"/>
     <sheet name="Table2" sheetId="5" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <definedNames>
     <definedName name="ColType">Definitions!$A$2:$A$6</definedName>
     <definedName name="MeasurandType">Definitions!$C$2:$C$152</definedName>
     <definedName name="MetaType">Definitions!$B$2:$B$21</definedName>
+    <definedName name="rgKommentar">[1]ODBC!$O$7:$P$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="432">
   <si>
     <t>customerTag</t>
   </si>
@@ -207,9 +211,6 @@
     <t>DCCTable</t>
   </si>
   <si>
-    <t>refID</t>
-  </si>
-  <si>
     <t>humanHeading</t>
   </si>
   <si>
@@ -465,12 +466,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>countryCodeISO3166_1</t>
-  </si>
-  <si>
-    <t>convention</t>
-  </si>
-  <si>
     <t>traceable</t>
   </si>
   <si>
@@ -1191,15 +1186,6 @@
     <t>TempCal</t>
   </si>
   <si>
-    <t>itemID</t>
-  </si>
-  <si>
-    <t>tableID</t>
-  </si>
-  <si>
-    <t>settingID</t>
-  </si>
-  <si>
     <t>setting01</t>
   </si>
   <si>
@@ -1264,6 +1250,102 @@
   </si>
   <si>
     <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:coreData/dcc:performanceLocation</t>
+  </si>
+  <si>
+    <t>255</t>
+  </si>
+  <si>
+    <t>DANAK</t>
+  </si>
+  <si>
+    <t>itemID1 itemID2</t>
+  </si>
+  <si>
+    <t>itemRef</t>
+  </si>
+  <si>
+    <t>settingRef</t>
+  </si>
+  <si>
+    <t>statementRef</t>
+  </si>
+  <si>
+    <t>tableId</t>
+  </si>
+  <si>
+    <t>statement</t>
+  </si>
+  <si>
+    <t>statement02</t>
+  </si>
+  <si>
+    <t>statement03</t>
+  </si>
+  <si>
+    <t>exceptionRef</t>
+  </si>
+  <si>
+    <t>exception01 exception02</t>
+  </si>
+  <si>
+    <t>Moonphase</t>
+  </si>
+  <si>
+    <t>Measurements marked in exception column refering to this exception were carried out at half moon.</t>
+  </si>
+  <si>
+    <t>Measurements marked in exception column refering to this exception were carried out at new moon.</t>
+  </si>
+  <si>
+    <t>Exception</t>
+  </si>
+  <si>
+    <t>Exception applies</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>e01</t>
+  </si>
+  <si>
+    <t>e02</t>
+  </si>
+  <si>
+    <t>e03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data marked with reference to this exception has increased uncertainty relative to the laboratory's best measurement capability  due to ill condition of the calibrated item. </t>
+  </si>
+  <si>
+    <t>exception</t>
+  </si>
+  <si>
+    <t>Excerpts of this report may only be reproduced with the written permission of the calibration laboratory.</t>
+  </si>
+  <si>
+    <t>name en</t>
+  </si>
+  <si>
+    <t>name da</t>
+  </si>
+  <si>
+    <t>Månefase</t>
+  </si>
+  <si>
+    <t>Unless otherwise stated, the measurements were caried out at full moon. I.e. $M&gt;=0.95M_{max}$.</t>
+  </si>
+  <si>
+    <t>description da</t>
+  </si>
+  <si>
+    <t>Med mindre andet er oplyst er alle målinger udført ved fuldmåne. Dvs: $M&gt;=0.95M_{max}$.</t>
+  </si>
+  <si>
+    <t>Reprint</t>
+  </si>
+  <si>
+    <t>Gengivelse af rapport i uddrag</t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1558,7 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1562,6 +1644,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
@@ -1569,7 +1657,20 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1637,8 +1738,163 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Januar"/>
+      <sheetName val="Februar"/>
+      <sheetName val="Marts"/>
+      <sheetName val="April"/>
+      <sheetName val="Maj"/>
+      <sheetName val="Juni"/>
+      <sheetName val="Juli"/>
+      <sheetName val="August"/>
+      <sheetName val="September"/>
+      <sheetName val="Oktober"/>
+      <sheetName val="November"/>
+      <sheetName val="December"/>
+      <sheetName val="Totaler"/>
+      <sheetName val="Vejledning"/>
+      <sheetName val="Balance"/>
+      <sheetName val="ODBC"/>
+      <sheetName val="Sagsdata"/>
+      <sheetName val="Aktivitet"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15">
+        <row r="7">
+          <cell r="O7" t="str">
+            <v>0212-01</v>
+          </cell>
+          <cell r="P7" t="str">
+            <v>CMM kunder</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="O8" t="str">
+            <v>0305-01</v>
+          </cell>
+          <cell r="P8" t="str">
+            <v>DANAK TA kursus (30t) + TA videnhjemtagning (10t)</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="O9" t="str">
+            <v>0501-01</v>
+          </cell>
+          <cell r="P9" t="str">
+            <v>korrektur + interne audits</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="O10" t="str">
+            <v>1000-01</v>
+          </cell>
+          <cell r="P10" t="str">
+            <v>230429JHA: Reduceret med 86t til at dække underbooking</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="O11" t="str">
+            <v>1107-04</v>
+          </cell>
+          <cell r="P11" t="str">
+            <v>Vedligehold (60 h), Sammenligning (28 h)</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="O12" t="str">
+            <v>1901-03</v>
+          </cell>
+          <cell r="P12" t="str">
+            <v>KMM opgave (200 h) 230508JHA: reduceret 20t</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="O13" t="str">
+            <v>2908-01</v>
+          </cell>
+          <cell r="P13" t="str">
+            <v xml:space="preserve">TKAK 15, Eurolab DK 15, FVM 60, </v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="O14" t="str">
+            <v>2910-01</v>
+          </cell>
+          <cell r="P14" t="str">
+            <v>EMPIR hjemmeside</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="O15" t="str">
+            <v>4005-02-01</v>
+          </cell>
+          <cell r="P15" t="str">
+            <v>primary conductivity cell</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="O16" t="str">
+            <v>4006-03</v>
+          </cell>
+          <cell r="P16" t="str">
+            <v xml:space="preserve">Digital Cal. Cert. (200 h), </v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="O17" t="str">
+            <v>7709-01</v>
+          </cell>
+          <cell r="P17" t="str">
+            <v>SRK har brugt 40t mod budgetteret 18t I Q2. Reduceret I Q3</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="O18" t="str">
+            <v>9211-16</v>
+          </cell>
+          <cell r="P18" t="str">
+            <v>230427JHA: Sum 100</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="O19" t="str">
+            <v>9441-02</v>
+          </cell>
+          <cell r="P19" t="str">
+            <v>Mission booster</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B1D61B28-1FF3-42F7-84C3-D339206597FD}" name="Table14" displayName="Table14" ref="A1:H6" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B1D61B28-1FF3-42F7-84C3-D339206597FD}" name="Table14" displayName="Table14" ref="A1:H6" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:H6" xr:uid="{B1D61B28-1FF3-42F7-84C3-D339206597FD}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{50EB9A61-D5FF-442A-A238-F83BEEC1CDAB}" name="swID"/>
@@ -1655,15 +1911,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0BCFA805-76BF-4AFE-9513-65BAFBCB25EE}" name="Table13" displayName="Table13" ref="A1:R6" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:R6" xr:uid="{0BCFA805-76BF-4AFE-9513-65BAFBCB25EE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0BCFA805-76BF-4AFE-9513-65BAFBCB25EE}" name="Table13" displayName="Table13" ref="B1:S7" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="B1:S7" xr:uid="{0BCFA805-76BF-4AFE-9513-65BAFBCB25EE}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{7378B2CC-F29E-41D1-9E44-CB13F033ED00}" name="id"/>
-    <tableColumn id="2" xr3:uid="{143B470D-A4E9-44CD-A4A5-F41E327CDC78}" name="refID"/>
-    <tableColumn id="3" xr3:uid="{E716D0AF-CFBE-4987-A1B3-355E26E44BC4}" name="name"/>
-    <tableColumn id="4" xr3:uid="{5A708E13-BA26-40AC-A0E0-AC3B29EF5716}" name="description"/>
-    <tableColumn id="5" xr3:uid="{902EAD39-1780-4DC5-A42D-B2BEFB319EC4}" name="countryCodeISO3166_1"/>
-    <tableColumn id="6" xr3:uid="{7652A258-98BD-42AE-BCD8-97C96C4CDD8C}" name="convention"/>
+    <tableColumn id="2" xr3:uid="{143B470D-A4E9-44CD-A4A5-F41E327CDC78}" name="exceptionRef"/>
+    <tableColumn id="3" xr3:uid="{E716D0AF-CFBE-4987-A1B3-355E26E44BC4}" name="name en"/>
+    <tableColumn id="4" xr3:uid="{5A708E13-BA26-40AC-A0E0-AC3B29EF5716}" name="description" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{902EAD39-1780-4DC5-A42D-B2BEFB319EC4}" name="name da"/>
+    <tableColumn id="6" xr3:uid="{7652A258-98BD-42AE-BCD8-97C96C4CDD8C}" name="description da"/>
     <tableColumn id="7" xr3:uid="{71043BA0-DD12-45DC-A3E5-6FC2F64A8D55}" name="traceable"/>
     <tableColumn id="8" xr3:uid="{3A28F3D9-4A81-401D-8FAB-72B24E0B7AEE}" name="norm"/>
     <tableColumn id="9" xr3:uid="{739F67C5-AB08-453B-8A10-F2E4E5B1C29B}" name="reference"/>
@@ -1682,7 +1938,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FC044B5-24CB-4140-A183-70424C80E6A8}" name="Table1" displayName="Table1" ref="A1:I6" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FC044B5-24CB-4140-A183-70424C80E6A8}" name="Table1" displayName="Table1" ref="A1:I6" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:I6" xr:uid="{2FC044B5-24CB-4140-A183-70424C80E6A8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{9BE8681D-A525-4CE6-BBF0-09C6834C3F35}" name="id"/>
@@ -1998,8 +2254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F9C957-7C4E-4161-9FBF-0EC69D9D67E3}">
   <dimension ref="A1:L152"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="C144" sqref="C144"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2013,19 +2269,19 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2036,10 +2292,10 @@
         <v>41</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="L2" s="2"/>
     </row>
@@ -2051,10 +2307,10 @@
         <v>37</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="L3" s="2"/>
     </row>
@@ -2066,10 +2322,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D4" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="L4" s="2"/>
     </row>
@@ -2081,10 +2337,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="L5" s="2"/>
     </row>
@@ -2093,7 +2349,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
@@ -2106,10 +2362,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D7" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="L7" s="2"/>
     </row>
@@ -2118,10 +2374,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D8" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="L8" s="2"/>
     </row>
@@ -2130,10 +2386,10 @@
         <v>38</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D9" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="L9" s="2"/>
     </row>
@@ -2142,10 +2398,10 @@
         <v>39</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D10" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="L10" s="2"/>
     </row>
@@ -2154,10 +2410,10 @@
         <v>40</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D11" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -2166,10 +2422,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D12" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="L12" s="2"/>
     </row>
@@ -2178,10 +2434,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D13" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="L13" s="2"/>
     </row>
@@ -2190,10 +2446,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D14" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="L14" s="2"/>
     </row>
@@ -2202,10 +2458,10 @@
         <v>31</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D15" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="L15" s="2"/>
     </row>
@@ -2214,105 +2470,108 @@
         <v>36</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D16" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D17" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D18" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D19" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="20" spans="2:4">
+      <c r="B20" t="s">
+        <v>415</v>
+      </c>
       <c r="C20" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D20" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="C21" s="31" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D21" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="C22" s="31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D22" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="C23" s="31" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D23" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="C24" s="31" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D24" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="C25" s="31" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D25" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="C26" s="31" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D26" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="C27" s="31" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D27" t="s">
         <v>50</v>
@@ -2320,39 +2579,39 @@
     </row>
     <row r="28" spans="2:4">
       <c r="C28" s="31" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D28" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="C29" s="31" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D29" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="C30" s="31" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D30" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="C31" s="31" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D31" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="C32" s="31" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D32" t="s">
         <v>48</v>
@@ -2360,637 +2619,637 @@
     </row>
     <row r="33" spans="3:4">
       <c r="C33" s="31" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D33" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="34" spans="3:4">
       <c r="C34" s="31" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D34" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="35" spans="3:4">
       <c r="C35" s="31" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D35" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="36" spans="3:4">
       <c r="C36" s="31" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D36" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" s="31" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D37" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="38" spans="3:4">
       <c r="C38" s="31" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D38" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="39" spans="3:4">
       <c r="C39" s="31" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D39" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="31" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D40" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="31" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D41" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="42" spans="3:4">
       <c r="C42" s="31" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D42" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="43" spans="3:4">
       <c r="C43" s="31" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D43" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="44" spans="3:4">
       <c r="C44" s="31" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D44" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="45" spans="3:4">
       <c r="C45" s="31" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D45" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="46" spans="3:4">
       <c r="C46" s="31" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D46" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="47" spans="3:4">
       <c r="C47" s="31" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D47" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="48" spans="3:4">
       <c r="C48" s="31" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D48" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D49" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" s="31" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D50" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="C51" s="31" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D51" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="C52" s="31" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D52" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="53" spans="3:4">
       <c r="C53" s="31" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D53" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="54" spans="3:4">
       <c r="C54" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D54" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="55" spans="3:4">
       <c r="C55" s="31" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D55" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="56" spans="3:4">
       <c r="C56" s="31" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D56" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="57" spans="3:4">
       <c r="C57" s="31" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D57" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="31" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D58" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" s="31" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D59" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="60" spans="3:4">
       <c r="C60" s="31" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D60" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" s="31" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D61" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="62" spans="3:4">
       <c r="C62" s="31" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D62" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="63" spans="3:4">
       <c r="C63" s="31" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D63" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="64" spans="3:4">
       <c r="C64" s="31" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D64" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" s="31" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D65" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="31" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D66" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" s="31" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D67" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="31" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" s="31" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="31" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="31" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="C72" s="31" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="31" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="C74" s="31" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="C75" s="31" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" s="31" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" s="31" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="31" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="31" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="80" spans="3:4">
       <c r="C80" s="31" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" s="31" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" s="31" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" s="31" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" s="31" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" s="31" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" s="31" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" s="31" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" s="31" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" s="31" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" s="31" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" s="31" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" s="31" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" s="31" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" s="31" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" s="31" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" s="31" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" s="31" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="98" spans="3:3">
       <c r="C98" s="31" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="99" spans="3:3">
       <c r="C99" s="31" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="100" spans="3:3">
       <c r="C100" s="31" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101" s="31" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="102" spans="3:3">
       <c r="C102" s="31" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="103" spans="3:3">
       <c r="C103" s="31" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="104" spans="3:3">
       <c r="C104" s="31" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="105" spans="3:3">
       <c r="C105" s="31" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="106" spans="3:3">
       <c r="C106" s="31" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="107" spans="3:3">
       <c r="C107" s="31" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="108" spans="3:3">
       <c r="C108" s="31" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="109" spans="3:3">
       <c r="C109" s="31" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="110" spans="3:3">
       <c r="C110" s="31" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="111" spans="3:3">
       <c r="C111" s="31" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="112" spans="3:3">
       <c r="C112" s="31" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="113" spans="3:3">
       <c r="C113" s="31" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="114" spans="3:3">
       <c r="C114" s="31" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="115" spans="3:3">
       <c r="C115" s="31" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="116" spans="3:3">
       <c r="C116" s="31" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="117" spans="3:3">
       <c r="C117" s="31" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="118" spans="3:3">
       <c r="C118" s="31" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="119" spans="3:3">
       <c r="C119" s="31" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="120" spans="3:3">
       <c r="C120" s="31" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="121" spans="3:3">
       <c r="C121" s="31" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="122" spans="3:3">
       <c r="C122" s="31" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="123" spans="3:3">
       <c r="C123" s="31" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="124" spans="3:3">
       <c r="C124" s="31" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="125" spans="3:3">
       <c r="C125" s="31" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="126" spans="3:3">
       <c r="C126" s="31" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="127" spans="3:3">
       <c r="C127" s="31" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="128" spans="3:3">
       <c r="C128" s="31" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="129" spans="3:3">
       <c r="C129" s="31" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="130" spans="3:3">
       <c r="C130" s="31" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="131" spans="3:3">
       <c r="C131" s="31" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="132" spans="3:3">
       <c r="C132" s="31" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="133" spans="3:3">
       <c r="C133" s="31" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="134" spans="3:3">
       <c r="C134" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
     </row>
     <row r="135" spans="3:3">
       <c r="C135" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="136" spans="3:3">
       <c r="C136" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
     </row>
     <row r="137" spans="3:3">
       <c r="C137" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
     </row>
     <row r="138" spans="3:3">
       <c r="C138" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
     <row r="139" spans="3:3">
@@ -3209,7 +3468,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3221,335 +3480,345 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
         <v>76</v>
       </c>
-      <c r="C2" t="s">
-        <v>77</v>
-      </c>
       <c r="D2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" t="s">
-        <v>79</v>
-      </c>
       <c r="D3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>81</v>
-      </c>
       <c r="D4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="28" t="s">
-        <v>84</v>
-      </c>
       <c r="D5" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="28" t="s">
-        <v>86</v>
-      </c>
       <c r="D6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>88</v>
-      </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" t="s">
         <v>89</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>91</v>
-      </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="D9" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="D10" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
         <v>93</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>94</v>
       </c>
-      <c r="C11" t="s">
-        <v>95</v>
-      </c>
       <c r="D11" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>97</v>
-      </c>
       <c r="D12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>99</v>
-      </c>
       <c r="D13" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" t="s">
         <v>100</v>
       </c>
-      <c r="C14" t="s">
-        <v>101</v>
-      </c>
       <c r="D14" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" t="s">
         <v>102</v>
       </c>
-      <c r="C15" t="s">
-        <v>103</v>
-      </c>
       <c r="D15" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="28" t="s">
-        <v>105</v>
-      </c>
       <c r="D16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="D17" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="30" t="s">
-        <v>108</v>
-      </c>
       <c r="D18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>110</v>
-      </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="C20" s="28" t="s">
-        <v>112</v>
-      </c>
       <c r="D20" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" t="s">
         <v>113</v>
       </c>
-      <c r="C21" t="s">
-        <v>114</v>
-      </c>
       <c r="D21" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" t="s">
         <v>126</v>
       </c>
-      <c r="C22" t="s">
-        <v>127</v>
-      </c>
       <c r="D22" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>116</v>
-      </c>
       <c r="D23" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="28" t="s">
-        <v>118</v>
-      </c>
       <c r="D24" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="C25" s="28"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D26" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="C27" s="28" t="s">
-        <v>121</v>
-      </c>
       <c r="D27" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" t="s">
         <v>122</v>
       </c>
-      <c r="C28" t="s">
-        <v>123</v>
-      </c>
       <c r="D28" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="C29" s="28" t="s">
-        <v>125</v>
-      </c>
       <c r="D29" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="C30" s="28"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="C31" s="28" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="C32" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="33" spans="3:3">
       <c r="C33" s="28"/>
@@ -3617,28 +3886,28 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>181</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -3652,94 +3921,177 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C531791-9242-4867-B027-97236DF4A138}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="3" t="s">
-        <v>129</v>
-      </c>
+    <row r="1" spans="1:20">
       <c r="B1" s="3" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="S1" s="3"/>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="T1" s="3"/>
+    </row>
+    <row r="2" spans="1:20" ht="75">
+      <c r="A2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C2" t="s">
+        <v>411</v>
+      </c>
+      <c r="D2" t="s">
+        <v>412</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>427</v>
+      </c>
+      <c r="F2" t="s">
+        <v>426</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="45">
+      <c r="A3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D3" t="s">
+        <v>430</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>423</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>394</v>
+        <v>407</v>
+      </c>
+      <c r="B4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="45">
+      <c r="A5" t="s">
+        <v>422</v>
+      </c>
+      <c r="B5" t="s">
+        <v>418</v>
+      </c>
+      <c r="C5" t="s">
+        <v>388</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="45">
+      <c r="A6" t="s">
+        <v>422</v>
+      </c>
+      <c r="B6" t="s">
+        <v>419</v>
+      </c>
+      <c r="C6" t="s">
+        <v>388</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="75">
+      <c r="A7" t="s">
+        <v>422</v>
+      </c>
+      <c r="B7" t="s">
+        <v>420</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -3755,8 +4107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181308C0-D531-4746-B510-8FF554CEB31C}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3773,61 +4125,61 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" t="s">
         <v>379</v>
       </c>
-      <c r="B2" t="s">
-        <v>385</v>
-      </c>
       <c r="C2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="F2" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="G2" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H2">
         <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3840,10 +4192,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C24526-8286-4257-8B46-E195D4F721E3}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3863,484 +4215,524 @@
     <col min="13" max="13" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17.25" customHeight="1">
+    <row r="2" spans="1:14" ht="17.25" customHeight="1">
       <c r="A2" s="27" t="s">
-        <v>382</v>
+        <v>406</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="27" t="s">
-        <v>381</v>
+        <v>403</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="27" t="s">
-        <v>383</v>
+        <v>404</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="27" t="s">
+        <v>405</v>
+      </c>
+      <c r="B5" s="27"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="27">
+        <f>COUNTA(A14:A1048576)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="27">
-        <f>COUNTA(A12:A1048576)</f>
+      <c r="B8" s="27">
+        <f>COUNTA(B9:XFD9)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="23.25">
+      <c r="A10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="27">
-        <f>COUNTA(B7:XFD7)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="1" t="s">
+      <c r="K10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="23.25">
+      <c r="A11" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="23.25">
-      <c r="A8" s="1" t="s">
+      <c r="B11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="23.25">
+      <c r="A12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>374</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="45.75">
+      <c r="A13" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="M13" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="N13" s="23" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="18">
         <v>0</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="23.25">
-      <c r="A9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="23.25">
-      <c r="A10" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="45.75">
-      <c r="A11" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="L11" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="M11" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="5" t="s">
+      <c r="D14" s="19">
+        <f>ROUND(E14+273.15,2)</f>
+        <v>273.16000000000003</v>
+      </c>
+      <c r="E14" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="F14" s="9">
+        <v>-0.1</v>
+      </c>
+      <c r="G14" s="9">
+        <f>ROUND(F14-E14,1)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="H14" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="I14" s="26">
+        <v>2</v>
+      </c>
+      <c r="J14" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L14" s="8">
+        <v>1</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="18">
-        <v>0</v>
-      </c>
-      <c r="D12" s="19">
-        <f>ROUND(E12+273.15,2)</f>
-        <v>273.16000000000003</v>
-      </c>
-      <c r="E12" s="19">
-        <v>0.01</v>
-      </c>
-      <c r="F12" s="9">
-        <v>-0.1</v>
-      </c>
-      <c r="G12" s="9">
-        <f>ROUND(F12-E12,1)</f>
-        <v>-0.1</v>
-      </c>
-      <c r="H12" s="25">
+      <c r="B15" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="18">
+        <v>15</v>
+      </c>
+      <c r="D15" s="19">
+        <f t="shared" ref="D15:D18" si="0">ROUND(E15+273.15,2)</f>
+        <v>288.16000000000003</v>
+      </c>
+      <c r="E15" s="19">
+        <v>15.01</v>
+      </c>
+      <c r="F15" s="9">
+        <v>15.1</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" ref="G15:G18" si="1">ROUND(F15-E15,1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="25">
         <v>0.05</v>
       </c>
-      <c r="I12" s="26">
+      <c r="I15" s="26">
         <v>2</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J15" s="9">
         <v>0.2</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K15" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="L12" s="8">
-        <v>1</v>
-      </c>
-      <c r="M12" s="9" t="s">
+      <c r="L15" s="8">
+        <v>2</v>
+      </c>
+      <c r="M15" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="6" t="s">
+      <c r="N15" s="9" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="18">
-        <v>15</v>
-      </c>
-      <c r="D13" s="19">
-        <f t="shared" ref="D13:D16" si="0">ROUND(E13+273.15,2)</f>
-        <v>288.16000000000003</v>
-      </c>
-      <c r="E13" s="19">
-        <v>15.01</v>
-      </c>
-      <c r="F13" s="9">
-        <v>15.1</v>
-      </c>
-      <c r="G13" s="9">
-        <f t="shared" ref="G13:G16" si="1">ROUND(F13-E13,1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="H13" s="25">
-        <v>0.05</v>
-      </c>
-      <c r="I13" s="26">
-        <v>2</v>
-      </c>
-      <c r="J13" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="L13" s="8">
-        <v>2</v>
-      </c>
-      <c r="M13" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="17" t="s">
+      <c r="B16" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C16" s="18">
         <v>25</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D16" s="19">
         <f t="shared" si="0"/>
         <v>298.17</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E16" s="19">
         <v>25.02</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F16" s="9">
         <v>25.2</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G16" s="9">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H16" s="25">
         <v>0.05</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I16" s="26">
         <v>2</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J16" s="9">
         <v>0.2</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K16" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L16" s="8">
         <v>3</v>
       </c>
-      <c r="M14" s="9" t="s">
+      <c r="M16" s="9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="17" t="s">
+      <c r="N16" s="9" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C17" s="18">
         <v>15</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D17" s="19">
         <f t="shared" si="0"/>
         <v>288.16000000000003</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E17" s="19">
         <v>15.01</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F17" s="9">
         <v>15.3</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G17" s="9">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H17" s="25">
         <v>0.05</v>
       </c>
-      <c r="I15" s="26">
+      <c r="I17" s="26">
         <v>2</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J17" s="9">
         <v>0.2</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K17" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="L15" s="8">
+      <c r="L17" s="8">
         <v>4</v>
       </c>
-      <c r="M15" s="9" t="s">
+      <c r="M17" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="20" t="s">
+      <c r="N17" s="9" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C18" s="21">
         <v>0</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D18" s="19">
         <f t="shared" si="0"/>
         <v>273.16000000000003</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E18" s="22">
         <v>0.01</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F18" s="7">
         <v>0</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G18" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H18" s="25">
         <v>0.05</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I18" s="26">
         <v>2</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J18" s="7">
         <v>0.2</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="K18" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L18" s="4">
         <v>5</v>
       </c>
-      <c r="M16" s="7" t="s">
+      <c r="M18" s="7" t="s">
         <v>43</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>419</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:M9" xr:uid="{01692EB9-2CFF-4754-B166-4E8AFE51A7B5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:N11" xr:uid="{01692EB9-2CFF-4754-B166-4E8AFE51A7B5}">
       <formula1>MeasurandType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:M7" xr:uid="{75EA51A4-45EC-43B4-8728-0EBA51E434E4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:N9" xr:uid="{75EA51A4-45EC-43B4-8728-0EBA51E434E4}">
       <formula1>ColType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:M8" xr:uid="{05FBC35F-3A35-49D1-B65B-475EDB16B6B1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:N10" xr:uid="{05FBC35F-3A35-49D1-B65B-475EDB16B6B1}">
       <formula1>MetaType</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add excel sheet with button to look up results
The sheet calls the script writetolookup.py
</commit_message>
<xml_diff>
--- a/DCC-Table_example3.xlsx
+++ b/DCC-Table_example3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\MS\4006-03 AI metrologi\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09607813-8499-453E-942B-3CB7332DBBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCCA27B-D95B-4B85-9232-E09009B60654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="2640" windowWidth="33540" windowHeight="12615" activeTab="3" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
+    <workbookView xWindow="3855" yWindow="2640" windowWidth="33540" windowHeight="12615" activeTab="5" xr2:uid="{7B806C36-EFAF-4198-BA2F-F0EE1FD641A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="430">
   <si>
     <t>customerTag</t>
   </si>
@@ -103,9 +103,6 @@
     <t>volumeRelative</t>
   </si>
   <si>
-    <t>\degreecelcius</t>
-  </si>
-  <si>
     <t>\kelvin</t>
   </si>
   <si>
@@ -1301,9 +1298,6 @@
   </si>
   <si>
     <t>Exception applies</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>e01</t>
@@ -2269,78 +2263,78 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L5" s="2"/>
     </row>
@@ -2349,10 +2343,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="2"/>
     </row>
@@ -2362,10 +2356,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L7" s="2"/>
     </row>
@@ -2374,46 +2368,46 @@
         <v>6</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12">
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12">
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -2422,10 +2416,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L12" s="2"/>
     </row>
@@ -2434,10 +2428,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L13" s="2"/>
     </row>
@@ -2446,810 +2440,810 @@
         <v>0</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12">
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12">
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D16" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D20" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="C21" s="31" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D21" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="C22" s="31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D22" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="C23" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="C24" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="C25" s="31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="C26" s="31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D26" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="C27" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="C28" s="31" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="C29" s="31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="C30" s="31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D30" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="C31" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D31" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="C32" s="31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="3:4">
       <c r="C33" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D33" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="34" spans="3:4">
       <c r="C34" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D34" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="35" spans="3:4">
       <c r="C35" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D35" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="36" spans="3:4">
       <c r="C36" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D36" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D37" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="38" spans="3:4">
       <c r="C38" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D38" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="39" spans="3:4">
       <c r="C39" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D39" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D40" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D41" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="42" spans="3:4">
       <c r="C42" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D42" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="43" spans="3:4">
       <c r="C43" s="31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D43" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="44" spans="3:4">
       <c r="C44" s="31" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D44" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="45" spans="3:4">
       <c r="C45" s="31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="46" spans="3:4">
       <c r="C46" s="31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D46" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="47" spans="3:4">
       <c r="C47" s="31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D47" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="48" spans="3:4">
       <c r="C48" s="31" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D48" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D49" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" s="31" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D50" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="C51" s="31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D51" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="C52" s="31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D52" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="53" spans="3:4">
       <c r="C53" s="31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D53" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="54" spans="3:4">
       <c r="C54" s="31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D54" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="55" spans="3:4">
       <c r="C55" s="31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D55" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="56" spans="3:4">
       <c r="C56" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D56" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="57" spans="3:4">
       <c r="C57" s="31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D57" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D58" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" s="31" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D59" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="60" spans="3:4">
       <c r="C60" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D60" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D61" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="62" spans="3:4">
       <c r="C62" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D62" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="63" spans="3:4">
       <c r="C63" s="31" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D63" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="64" spans="3:4">
       <c r="C64" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D64" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" s="31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D65" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D66" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D67" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" s="31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="C72" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="C74" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="C75" s="31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="80" spans="3:4">
       <c r="C80" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" s="31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" s="31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" s="31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" s="31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" s="31" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" s="31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" s="31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" s="31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="98" spans="3:3">
       <c r="C98" s="31" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="99" spans="3:3">
       <c r="C99" s="31" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="100" spans="3:3">
       <c r="C100" s="31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101" s="31" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="102" spans="3:3">
       <c r="C102" s="31" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="103" spans="3:3">
       <c r="C103" s="31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="104" spans="3:3">
       <c r="C104" s="31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="105" spans="3:3">
       <c r="C105" s="31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="106" spans="3:3">
       <c r="C106" s="31" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="107" spans="3:3">
       <c r="C107" s="31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="108" spans="3:3">
       <c r="C108" s="31" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="109" spans="3:3">
       <c r="C109" s="31" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="110" spans="3:3">
       <c r="C110" s="31" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="111" spans="3:3">
       <c r="C111" s="31" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="112" spans="3:3">
       <c r="C112" s="31" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="113" spans="3:3">
       <c r="C113" s="31" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="114" spans="3:3">
       <c r="C114" s="31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="115" spans="3:3">
       <c r="C115" s="31" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="116" spans="3:3">
       <c r="C116" s="31" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="117" spans="3:3">
       <c r="C117" s="31" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="118" spans="3:3">
       <c r="C118" s="31" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="119" spans="3:3">
       <c r="C119" s="31" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="120" spans="3:3">
       <c r="C120" s="31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="121" spans="3:3">
       <c r="C121" s="31" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="122" spans="3:3">
       <c r="C122" s="31" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="123" spans="3:3">
       <c r="C123" s="31" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="124" spans="3:3">
       <c r="C124" s="31" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="125" spans="3:3">
       <c r="C125" s="31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="126" spans="3:3">
       <c r="C126" s="31" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="127" spans="3:3">
       <c r="C127" s="31" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="128" spans="3:3">
       <c r="C128" s="31" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="129" spans="3:3">
       <c r="C129" s="31" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="130" spans="3:3">
       <c r="C130" s="31" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="131" spans="3:3">
       <c r="C131" s="31" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="132" spans="3:3">
       <c r="C132" s="31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="133" spans="3:3">
       <c r="C133" s="31" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="134" spans="3:3">
       <c r="C134" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="135" spans="3:3">
       <c r="C135" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="136" spans="3:3">
       <c r="C136" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="137" spans="3:3">
       <c r="C137" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="138" spans="3:3">
       <c r="C138" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="139" spans="3:3">
@@ -3304,22 +3298,22 @@
     </row>
     <row r="149" spans="3:3">
       <c r="C149" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="150" spans="3:3">
       <c r="C150" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="151" spans="3:3">
       <c r="C151" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="152" spans="3:3">
       <c r="C152" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -3480,344 +3474,344 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" t="s">
-        <v>76</v>
-      </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
         <v>77</v>
       </c>
-      <c r="C3" t="s">
-        <v>78</v>
-      </c>
       <c r="D3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>80</v>
-      </c>
       <c r="D4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="28" t="s">
-        <v>83</v>
-      </c>
       <c r="D5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="28" t="s">
-        <v>85</v>
-      </c>
       <c r="D6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>87</v>
-      </c>
       <c r="D7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
         <v>88</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>90</v>
-      </c>
       <c r="D8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="s">
+        <v>396</v>
+      </c>
+      <c r="C9" s="28" t="s">
         <v>397</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="D9" t="s">
         <v>398</v>
-      </c>
-      <c r="D9" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
+        <v>392</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>394</v>
+      </c>
+      <c r="D10" t="s">
         <v>393</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>395</v>
-      </c>
-      <c r="D10" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
         <v>92</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>93</v>
       </c>
-      <c r="C11" t="s">
-        <v>94</v>
-      </c>
       <c r="D11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>96</v>
-      </c>
       <c r="D12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>98</v>
-      </c>
       <c r="D13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" t="s">
         <v>99</v>
       </c>
-      <c r="C14" t="s">
-        <v>100</v>
-      </c>
       <c r="D14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" t="s">
         <v>101</v>
       </c>
-      <c r="C15" t="s">
-        <v>102</v>
-      </c>
       <c r="D15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="28" t="s">
-        <v>104</v>
-      </c>
       <c r="D16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="30" t="s">
-        <v>107</v>
-      </c>
       <c r="D18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="D19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="C20" s="28" t="s">
-        <v>111</v>
-      </c>
       <c r="D20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" t="s">
         <v>112</v>
       </c>
-      <c r="C21" t="s">
-        <v>113</v>
-      </c>
       <c r="D21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" t="s">
         <v>125</v>
       </c>
-      <c r="C22" t="s">
-        <v>126</v>
-      </c>
       <c r="D22" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>115</v>
-      </c>
       <c r="D23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="C24" s="28" t="s">
-        <v>117</v>
-      </c>
       <c r="D24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C25" s="28"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="C27" s="28" t="s">
-        <v>120</v>
-      </c>
       <c r="D27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" t="s">
         <v>121</v>
       </c>
-      <c r="C28" t="s">
-        <v>122</v>
-      </c>
       <c r="D28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="C29" s="28" t="s">
-        <v>124</v>
-      </c>
       <c r="D29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C30" s="28"/>
     </row>
     <row r="31" spans="2:4">
       <c r="C31" s="28" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="C32" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="33" spans="3:3">
@@ -3886,28 +3880,28 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>178</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -3923,7 +3917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C531791-9242-4867-B027-97236DF4A138}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -3952,146 +3946,146 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="B1" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="T1" s="3"/>
     </row>
     <row r="2" spans="1:20" ht="75">
       <c r="A2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D2" t="s">
         <v>411</v>
       </c>
-      <c r="D2" t="s">
-        <v>412</v>
-      </c>
       <c r="E2" s="34" t="s">
+        <v>425</v>
+      </c>
+      <c r="F2" t="s">
+        <v>424</v>
+      </c>
+      <c r="G2" s="34" t="s">
         <v>427</v>
-      </c>
-      <c r="F2" t="s">
-        <v>426</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="45">
       <c r="A3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B3" t="s">
         <v>407</v>
       </c>
-      <c r="B3" t="s">
-        <v>408</v>
-      </c>
       <c r="D3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="45">
       <c r="A5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="45">
       <c r="A6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="75">
       <c r="A7" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B7" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -4125,61 +4119,61 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C2" t="s">
+        <v>373</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
+        <v>373</v>
+      </c>
+      <c r="F2" t="s">
         <v>379</v>
       </c>
-      <c r="C2" t="s">
-        <v>374</v>
-      </c>
-      <c r="D2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" t="s">
-        <v>374</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>380</v>
-      </c>
-      <c r="G2" t="s">
-        <v>381</v>
       </c>
       <c r="H2">
         <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -4194,8 +4188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C24526-8286-4257-8B46-E195D4F721E3}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4217,36 +4211,36 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="17.25" customHeight="1">
       <c r="A2" s="27" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="27" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="27" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="27" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B5" s="27"/>
     </row>
@@ -4256,7 +4250,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="27">
         <f>COUNTA(A14:A1048576)</f>
@@ -4265,7 +4259,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="27">
         <f>COUNTA(B9:XFD9)</f>
@@ -4274,75 +4268,75 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="H9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>35</v>
-      </c>
       <c r="M9" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="23.25">
       <c r="A10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>62</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>63</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>5</v>
@@ -4354,150 +4348,150 @@
         <v>7</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="23.25">
       <c r="A11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="23.25">
       <c r="A12" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C12" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="E12" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="N12" s="15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="45.75">
       <c r="A13" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="23" t="s">
-        <v>21</v>
-      </c>
       <c r="F13" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I13" s="24" t="s">
-        <v>65</v>
-      </c>
       <c r="J13" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K13" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L13" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="M13" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="M13" s="23" t="s">
-        <v>71</v>
-      </c>
       <c r="N13" s="23" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="18">
         <v>0</v>
@@ -4526,24 +4520,24 @@
         <v>0.2</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L14" s="8">
         <v>1</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="18">
         <v>15</v>
@@ -4572,24 +4566,24 @@
         <v>0.2</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L15" s="8">
         <v>2</v>
       </c>
       <c r="M15" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N15" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="18">
         <v>25</v>
@@ -4618,24 +4612,24 @@
         <v>0.2</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L16" s="8">
         <v>3</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="18">
         <v>15</v>
@@ -4664,24 +4658,24 @@
         <v>0.2</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L17" s="8">
         <v>4</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="21">
         <v>0</v>
@@ -4710,16 +4704,16 @@
         <v>0.2</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L18" s="4">
         <v>5</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New filenames Update excel2dcc.py - new filename generated from CertID.
</commit_message>
<xml_diff>
--- a/DCC-Table_example3.xlsx
+++ b/DCC-Table_example3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tesla\Data\MS\4006-03 AI metrologi\Software\DCCtables\master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\1901 NY-INFRA-FOT\DCC\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3099841-3A4E-49A3-8D9A-A9935ADF6822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF9F7D7-C6EE-4686-BACD-5BCC5D44F83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="2460" windowWidth="32685" windowHeight="14520" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="37220" windowHeight="21820" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -18,19 +18,19 @@
     <sheet name="Software" sheetId="8" r:id="rId3"/>
     <sheet name="Statements" sheetId="6" r:id="rId4"/>
     <sheet name="Items" sheetId="7" r:id="rId5"/>
-    <sheet name="Table2" sheetId="5" r:id="rId6"/>
-    <sheet name="Settings" sheetId="9" r:id="rId7"/>
+    <sheet name="Settings" sheetId="9" r:id="rId6"/>
+    <sheet name="Table2" sheetId="5" r:id="rId7"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
-    <definedName name="ColType" localSheetId="6">[1]Definitions!$A$2:$A$6</definedName>
+    <definedName name="ColType" localSheetId="5">[1]Definitions!$A$2:$A$6</definedName>
     <definedName name="ColType">Definitions!$A$2:$A$6</definedName>
-    <definedName name="MeasurandType" localSheetId="6">[1]Definitions!$C$2:$C$152</definedName>
+    <definedName name="MeasurandType" localSheetId="5">[1]Definitions!$C$2:$C$152</definedName>
     <definedName name="MeasurandType">Definitions!$C$2:$C$152</definedName>
-    <definedName name="MetaType" localSheetId="6">[1]Definitions!$B$2:$B$21</definedName>
+    <definedName name="MetaType" localSheetId="5">[1]Definitions!$B$2:$B$21</definedName>
     <definedName name="MetaType">Definitions!$B$2:$B$21</definedName>
     <definedName name="rgKommentar">[2]ODBC!$O$7:$P$19</definedName>
   </definedNames>
@@ -3174,16 +3174,16 @@
   <dimension ref="A1:L152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -4391,11 +4391,11 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4793,16 +4793,16 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.81640625" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4849,27 +4849,27 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="34" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="5" width="41.453125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.26953125" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="9" max="9" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1796875" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="7.26953125" customWidth="1"/>
+    <col min="14" max="14" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -4929,7 +4929,7 @@
       </c>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="75">
+    <row r="2" spans="1:20" ht="72.5">
       <c r="A2" t="s">
         <v>405</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="75">
+    <row r="3" spans="1:20" ht="72.5">
       <c r="A3" t="s">
         <v>405</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="45">
+    <row r="5" spans="1:20" ht="43.5">
       <c r="A5" t="s">
         <v>419</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="45">
+    <row r="6" spans="1:20" ht="43.5">
       <c r="A6" t="s">
         <v>419</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="75">
+    <row r="7" spans="1:20" ht="58">
       <c r="A7" t="s">
         <v>419</v>
       </c>
@@ -5037,16 +5037,16 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" customWidth="1"/>
+    <col min="3" max="3" width="24.7265625" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="24.7265625" customWidth="1"/>
+    <col min="8" max="8" width="16.54296875" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -5143,29 +5143,219 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164255F3-93CF-4992-BB4A-5F2B2030CF33}">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="3" width="25.26953125" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" customWidth="1"/>
+    <col min="5" max="5" width="22.26953125" customWidth="1"/>
+    <col min="6" max="6" width="55.26953125" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>421</v>
+      </c>
+      <c r="D1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" t="s">
+        <v>422</v>
+      </c>
+      <c r="F1" t="s">
+        <v>425</v>
+      </c>
+      <c r="G1" t="s">
+        <v>445</v>
+      </c>
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>436</v>
+      </c>
+      <c r="B5" t="s">
+        <v>444</v>
+      </c>
+      <c r="C5" t="s">
+        <v>442</v>
+      </c>
+      <c r="D5" t="s">
+        <v>441</v>
+      </c>
+      <c r="E5" t="s">
+        <v>440</v>
+      </c>
+      <c r="F5" t="s">
+        <v>439</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>436</v>
+      </c>
+      <c r="B6" t="s">
+        <v>443</v>
+      </c>
+      <c r="C6" t="s">
+        <v>442</v>
+      </c>
+      <c r="D6" t="s">
+        <v>441</v>
+      </c>
+      <c r="E6" t="s">
+        <v>440</v>
+      </c>
+      <c r="F6" t="s">
+        <v>439</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>436</v>
+      </c>
+      <c r="B7" t="s">
+        <v>438</v>
+      </c>
+      <c r="C7" t="s">
+        <v>434</v>
+      </c>
+      <c r="D7" t="s">
+        <v>433</v>
+      </c>
+      <c r="E7" t="s">
+        <v>432</v>
+      </c>
+      <c r="F7" t="s">
+        <v>431</v>
+      </c>
+      <c r="G7">
+        <v>9.9</v>
+      </c>
+      <c r="H7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>436</v>
+      </c>
+      <c r="B8" t="s">
+        <v>437</v>
+      </c>
+      <c r="C8" t="s">
+        <v>434</v>
+      </c>
+      <c r="D8" t="s">
+        <v>433</v>
+      </c>
+      <c r="E8" t="s">
+        <v>432</v>
+      </c>
+      <c r="F8" t="s">
+        <v>431</v>
+      </c>
+      <c r="G8">
+        <v>0.99</v>
+      </c>
+      <c r="H8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>436</v>
+      </c>
+      <c r="B9" t="s">
+        <v>435</v>
+      </c>
+      <c r="C9" t="s">
+        <v>434</v>
+      </c>
+      <c r="D9" t="s">
+        <v>433</v>
+      </c>
+      <c r="E9" t="s">
+        <v>432</v>
+      </c>
+      <c r="F9" t="s">
+        <v>431</v>
+      </c>
+      <c r="G9">
+        <v>9.9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>436</v>
+      </c>
+      <c r="B10" t="s">
+        <v>446</v>
+      </c>
+      <c r="C10" t="s">
+        <v>447</v>
+      </c>
+      <c r="D10" t="s">
+        <v>448</v>
+      </c>
+      <c r="E10" t="s">
+        <v>449</v>
+      </c>
+      <c r="F10" t="s">
+        <v>450</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
+    <col min="10" max="10" width="14.54296875" customWidth="1"/>
+    <col min="11" max="11" width="13.7265625" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -5276,7 +5466,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="23.25">
+    <row r="10" spans="1:14" ht="22">
       <c r="A10" s="1" t="s">
         <v>68</v>
       </c>
@@ -5320,7 +5510,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="23.25">
+    <row r="11" spans="1:14" ht="22">
       <c r="A11" s="1" t="s">
         <v>67</v>
       </c>
@@ -5364,7 +5554,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="23.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="10" t="s">
         <v>53</v>
       </c>
@@ -5408,7 +5598,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="45.75">
+    <row r="13" spans="1:14" ht="32.5">
       <c r="A13" s="11" t="s">
         <v>52</v>
       </c>
@@ -5702,193 +5892,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164255F3-93CF-4992-BB4A-5F2B2030CF33}">
-  <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="55.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="B1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E1" t="s">
-        <v>422</v>
-      </c>
-      <c r="F1" t="s">
-        <v>425</v>
-      </c>
-      <c r="G1" t="s">
-        <v>445</v>
-      </c>
-      <c r="H1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>436</v>
-      </c>
-      <c r="B5" t="s">
-        <v>444</v>
-      </c>
-      <c r="C5" t="s">
-        <v>442</v>
-      </c>
-      <c r="D5" t="s">
-        <v>441</v>
-      </c>
-      <c r="E5" t="s">
-        <v>440</v>
-      </c>
-      <c r="F5" t="s">
-        <v>439</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>436</v>
-      </c>
-      <c r="B6" t="s">
-        <v>443</v>
-      </c>
-      <c r="C6" t="s">
-        <v>442</v>
-      </c>
-      <c r="D6" t="s">
-        <v>441</v>
-      </c>
-      <c r="E6" t="s">
-        <v>440</v>
-      </c>
-      <c r="F6" t="s">
-        <v>439</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>436</v>
-      </c>
-      <c r="B7" t="s">
-        <v>438</v>
-      </c>
-      <c r="C7" t="s">
-        <v>434</v>
-      </c>
-      <c r="D7" t="s">
-        <v>433</v>
-      </c>
-      <c r="E7" t="s">
-        <v>432</v>
-      </c>
-      <c r="F7" t="s">
-        <v>431</v>
-      </c>
-      <c r="G7">
-        <v>9.9</v>
-      </c>
-      <c r="H7" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>436</v>
-      </c>
-      <c r="B8" t="s">
-        <v>437</v>
-      </c>
-      <c r="C8" t="s">
-        <v>434</v>
-      </c>
-      <c r="D8" t="s">
-        <v>433</v>
-      </c>
-      <c r="E8" t="s">
-        <v>432</v>
-      </c>
-      <c r="F8" t="s">
-        <v>431</v>
-      </c>
-      <c r="G8">
-        <v>0.99</v>
-      </c>
-      <c r="H8" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>436</v>
-      </c>
-      <c r="B9" t="s">
-        <v>435</v>
-      </c>
-      <c r="C9" t="s">
-        <v>434</v>
-      </c>
-      <c r="D9" t="s">
-        <v>433</v>
-      </c>
-      <c r="E9" t="s">
-        <v>432</v>
-      </c>
-      <c r="F9" t="s">
-        <v>431</v>
-      </c>
-      <c r="G9">
-        <v>9.9</v>
-      </c>
-      <c r="H9" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>436</v>
-      </c>
-      <c r="B10" t="s">
-        <v>446</v>
-      </c>
-      <c r="C10" t="s">
-        <v>447</v>
-      </c>
-      <c r="D10" t="s">
-        <v>448</v>
-      </c>
-      <c r="E10" t="s">
-        <v>449</v>
-      </c>
-      <c r="F10" t="s">
-        <v>450</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>